<commit_message>
Updates and fix bugs
</commit_message>
<xml_diff>
--- a/SOP/Utterances/phrasesAgainstPositive.xlsx
+++ b/SOP/Utterances/phrasesAgainstPositive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marie\Desktop\Git\Storytelling_SR\SOP\Utterances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D5922C-14DF-477D-AFCD-5AEDD7E5FC56}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A8B733-C905-4971-9B71-AD12A7F2FD60}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24015" xr2:uid="{E4B8DB12-B672-4611-9817-EB9A51AE5FB6}"/>
   </bookViews>
@@ -282,28 +282,28 @@
     <t>EN:AGAINST</t>
   </si>
   <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Pessoalmente; esta é a minha decisão favorita.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Pessoalmente; prefiro a outra decisão.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Definitely; this will help people.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Wonderful. With this decision; you will save the people.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Personally; this is myfavourite decision.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Definitely; I disagree with you.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Wrong. With this decision; people will suffer.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Personally; I prefer other decision.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Definitely this will help people.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Wonderful. With this decision you will save the people.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Personally this is myfavourite decision.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Definitely I disagree with you.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Wrong. With this decision people will suffer.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Personally I prefer other decision.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Pessoalmente esta é a minha decisão favorita.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;  Pessoalmente prefiro a outra decisão.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
   </si>
 </sst>
 </file>
@@ -847,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC699C3-7B7D-494D-9389-830F8CDC6B9F}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="D55" sqref="D2:D65"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,7 +1040,7 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1236,7 +1236,7 @@
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1376,7 +1376,7 @@
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1404,7 +1404,7 @@
         <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1432,7 +1432,7 @@
         <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1586,7 +1586,7 @@
         <v>4</v>
       </c>
       <c r="D52" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1600,7 +1600,7 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1628,7 +1628,7 @@
         <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add robot side to log files
</commit_message>
<xml_diff>
--- a/SOP/Utterances/phrasesAgainstPositive.xlsx
+++ b/SOP/Utterances/phrasesAgainstPositive.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria José Ferreira\Desktop\GitStorytelling\SOP\Utterances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marie\Desktop\Git\Storytelling_SR\SOP\Utterances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EA79CC-7478-41D3-BE54-FC7E437969AD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF6AA79-6416-4E83-AEB9-31D327EBD4FA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11415" activeTab="2" xr2:uid="{44FFEBE6-F1D8-41FA-8CF8-D767FF193A3D}"/>
   </bookViews>
@@ -710,9 +710,6 @@
     <t>The ball is a great moment and the speech is really necessary to soften the independent concern when it happens.</t>
   </si>
   <si>
-    <t>As murálhas são o mais importante. Sem as muralhas o castelo ficará desprotegido contra grandes armas. Mude de decisão rapidamente.</t>
-  </si>
-  <si>
     <t>The gate is more important. It is the entrance to the castle, you have to prevent the enemies from entering. Change your decision quickly.</t>
   </si>
   <si>
@@ -825,6 +822,9 @@
   </si>
   <si>
     <t>Estou de acordo com esta decisão. Tens que confirmar esta opção para todos saberem.</t>
+  </si>
+  <si>
+    <t>As paredes são o mais importante. Sem as muralhas o castelo ficará desprotegido contra grandes armas. Mude de decisão rapidamente.</t>
   </si>
 </sst>
 </file>
@@ -1421,15 +1421,15 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.265625" customWidth="1"/>
-    <col min="3" max="3" width="15.1328125" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="219" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1445,7 +1445,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que irás ficar muito espouhsto. Muda de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a não fazer um baile neste momento, e sim a preparar-nos para uma batalha. Escolhe a outra opção.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que ao falares primeiro, podes influenciar os teus conselheiros. Deverias mudar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não deverias te expôr tanto, acho que deverias te retirar do baile. Pensa melhor e muda de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho que converses apenas com os nossos aliados mais antigos.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não te aconselho a deixar que alguém desconhecido entre. Isso é muito perigoso.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Este não é o momento de intérahgir com o adversário. Deverias mudar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho que solicites explicações imediatamente. Quanto mais cedo melhor para o país se preparar.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deixe o falar enquanto tentamos perceber melhor qual a tática dele. Deste modo, as defesas poderão ser preparadas melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Recomendo a agir rapidamente, pois precisamos de mais militares com urgência.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;A minha intuição diz-me que não há tempo para defender a rua principal. Com esta decisão, iremos perder muitos militares desnecessariamente.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que o mensageiro transmitiu a informação correta. Tens que demonstrar confiança no teu povo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a aproveitar esse tempo para enviar um batalhão de soldados para o ataque e acabar com o inimigo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a enviar uma tropa de soldados rapidamente para garantir a vitória e não deixar os aliados esperando. Pois, eles podem ir embora.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Com apenas metade dos soldados não acho que seremos vitoriósos. Acredito que os aliados não terão força suficiente para derrotar o inimigo. Pensa melhor e, muda de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a não sair da protéção da cidade por enquanto. Ainda é muito arriscado ir ao campo de batalha, podemos ser surpreendidos. Pensa melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não deves te expor ao inimigo desta forma. Além disso, fazer o primeiro contacto indica fraqueza. Pensa melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que deverias ser mais diplomático. Além disso, agradecer o convite é um sinal de educação.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Recomendo que mantenhas a tua liderança e jámais te rendas. Deverias mudar de decisão e mostrar a tua força.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acho que não deves mudar de opinião, pois isso demonstra fraquesa. Pensa melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que há várias maneiras para bloquear o acesso, devias pensar melhore trocar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;O sentimento de patriotismo é importante para incentivar o povo. Deverias mudar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não deves interagir com todos os conselheiros apenas um deve falar. Falar com todos vais ficar muito espouhsto, pode ser perigoso. Pensa melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que deverias falar em público, pois o teu povo precisa saber o que se passa. Muda de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a que organizes um baile para o teu povo ficar mais unido. Escolha a outra opção.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que deverias expressar primeiro a tua opinião. Deverias mudar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que deverias falar com todos no baile para mostrar que estás tranquilo com a situação. Não saia agora, mude de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que conversar com novos aliados trará novas ideias.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho que coñeças o mensageiro. Tens que ver a face do inimigo para conseguir vence-lo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deves tentar ganhar a confiança do adversário convidando-o. Deverias mudar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deverias ser mais gentil, e esperar que o adversário termine de falar. Ele não gosta de ser interrompido, sinto que isso pode apressar a batalha.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deves fazer o adversário parar de falar imediatamente. Acredito que ele quer descobrir algo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deves pensar melhor nesta intenção, pois a população pode ser muito afectada com esta decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a enviar imediatamente soldados para defender a rua. Com esta decisão, o castelo será tomado com maior facilidade pelo inimigo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Sinto que o inimigo não perdeu tanta força como informou o mensageiro. Pouco provável que o mensageiro conseguiria ter a informação correcta em um campo de batalha.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que deves pensar no nosso exército e deixá-lo descansar. Assim, novas estratégias de combate podem ser criadas sem muitas baixas.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Cuidado, se enviares as tropas podemos ficar sem soldados suficientes para nos proteger.  Devemos ter certeza que são aliados, pois podem ser inimigos.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Assim ficaremos fracos e desprutegidos. Acredito que os aliados podem conseguir derrotar o inimigo com metade dos nossos soldados e, ao mesmo tempo, estaremos protegidos. Pense melhor e, mude de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a ires pessoalmente e congratulá-lo pela vitória. Desse modo, mostrarás a todos que não tens medo de nada e de ninguém. Deverias pensar melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deves chamar o líder inimigo. Além disso, chamando ele indicas que ainda és forte. Pense melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que não deves mostrar diplomacia para com o inimigo. Além disso, o inimigo deve entender que ficamos indignados com a ameaça.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Devias negociar, pois o teu povo depende de ti. Deverias mudar de decisão e mostrar que se importas com o povo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que deves mudar de decisão, pois agora deves ter certeza da decisão. Pense melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que agora não há mais nada a fazer para defender o acesso. Estamos perdendo tempo ao pensar em novas ideias.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Agora não precisamos de símbolos, mas sim de ações. Deverias mudar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deverias saber a opinião de cada um dos membros do conselho. Assim todos vão se sentir importantes. Pense melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Esta é a melhor decisão a ser tomada, pois eles precisam saber primeiro. Confirme esta decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Eu gosto desta decisão, pois, é a melhor forma de estar pronto para uma batalha. Confirme-a.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Mantém essa decisão. Todos terão a sua vez de falar.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Estou de acordo com esta decisão. Acredito ser o melhor pra todos.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Entendo o teu ponto de vista e concordo. Aliados são bem vindos neste momento.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que tomastes a melhor decisão para este momento. A outra decisão irá gerar muitos problemas.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que esta decisão é a mais segura para o nosso povo. Confirme-a.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo com esta decisão. Assim, saberemos os motivos no momento ideal.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aprovo esta decisão, acredito que assim será melhor para o povo. Confirme-a.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que esta decisão é a mais sensata para o momento. Deves confirma-la.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que com esta decisão teremos mais vantagem. Vamos a isto.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Eu gosto desta decisão. De qualquer forma o inimigo está mais fraco.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que esta é a melhor estratégia para alcançar a vitória. Deves confirma-la.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo com esta decisão, é a mais sensata. Acredito que com isto caminhamos para a vitória.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que com esta decisão os aliados seremos todos vitóriosos. Deves confirma-la.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo contigo. Precisamos agradecer aos aliados de uma forma ou de outra.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo com a tua decisão, devemos diminuir o estrago da derrota. Deves confirmar esta decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aprovo esta decisão, devemos convidar o líder inimigo para nos visitar. Confirme e um mensageiro será enviado.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Apoiado. Acredito que todos irão entender esta decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo com esta decisão. Confirma-a.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Muito bem, apóio esta decisão. Deverias confirma-la imediatamente.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo que esta decisão é a mais correta para o momento.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que esta é a melhor forma de saber a opinião deles.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I think you will be very exposed. Change your decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise that this is not the time for a ball, but to prepare for a battle. Chose the other option.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that by speaking first you can influence your counselors.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should not expose yourself so much and you should withdraw from the ball. Think better, and change your decision. &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advice you just talk to our old allies.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I do not advise anyone unknown to come in. This is very dangerous.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;This is not the time to interact with the enemy. You should change the decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you to request explanations immediately. The sooner the better for the country to prepare.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Let him talk as we try to better understand his tactics. In this way, defenses can be better prepared.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Recommend to act quickly we need more military urgently.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;My intuition says there is no time to defend the main access. With this decision, we will lose many soldiers unnecessarily.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe the messenger has passed on the correct information. You have to show confidence in your people.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you to send a troop to the attack and finishing the enemy.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you to send a troop of soldiers quickly to ensure the victory and not leave the allies waiting. Because, they can leave.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;With only half the soldiers I do not think we will be victorious. I believe that the allies will not have enough strength to defeat the enemy. Think better, and change your mind.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you not to leave the protections of the city yet. It is still very risky to go to the battlefield, we may be surprised. Think better.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should not expose yourself to the enemy in this way. Also, making the first contact indicates weakness. Think better.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I think you should be more diplomatic. Also, thanking the invitation is a sign of education.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I recommend that you should be a leader and never surrender. You should change your mind and show your strength.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I do not think you should change your mind, because it shows weakness. You should think better.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that there are several ideas to block the accesses, you should think better and change your decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;The feeling of patriotism is important to encourage the people. You should change your decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should not interact with everyone on the council just one should talk. Talking to everyone will be very exposed, it can be dangerous. Think better.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that you should to speech to the public, they need to know. Change your decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you to organize the ball for the people to be more united.  Chose the other option.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that you should speak first of all to know your opinion.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I think you should talk to everyone at the ball to show peace. Do not leave now, change your decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that talking to new allies will bring new ideas.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you to meet this person. You have to see the enemy's face to defeat him.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should try to gain the confidence of the enemy by inviting him. You should change the decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should be kinder and wait for the enemy to finish talking. He does not like being interrupted, I feel that this can hasten the battle.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should immediately make him stop talking. I think he wants to find out something.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should think better about this intention because the population can be very affected whit this decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you to immediately send soldiers to defend access. With this decision, the castle will be taken more easily by the enemy.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I feel that the enemy has not lost as much force as the messenger informs. Unlikely the messenger would get the correct information on a battlefield.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I think you should think about our army and let them rest. Thus, new combat strategies can be created without many casualties.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Be careful, if you send the troops, we can run out of enough soldiers to protect us. We must be sure that allies, they can be enemies.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;That way we'll be weak and out of touch. I believe that the Allies can successfully defeat the enemy with half of our soldiers, and at the same time we will be protected. Think better, and change your mind.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you to go personally and congratulate them for the victory. In this way, you will show to everyone that you are not afraid of anything and nobody. You should think better.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should call the enemy leader. Also, calling him indicates that you're still strong. Think better.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I do not think you should show diplomacy to the enemy. In addition, the enemy must understand that we are outraged by the threat.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should trade, because your people depend on you. You should change your mind and show that you care about the people.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that you must change your decision, because now you are certain of the decision. You should think better.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that there is no longer any way to defend the access. We are wasting time thinking about new ideas.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;We do not need symbols, but actions. You should change your decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should know the opinion of each one of the council. So everyone will feel important. Think better.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;This is the best decision to be taken, because they need to know first.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I like this decision, because it is the best way to be ready for a battle. Confirm it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Keep that decision. Everyone will have their turn to speak.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with this decision. I believe that is the best for all.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I understand your point of view and agree with it. Allies are welcome at this time.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that you have made the best decision for this moment. The other decision will generate many problems.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that this decision is the safest for our people. Confirm it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with this decision. In this way, we will know the motives at the ideal moment.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I approve this decision, I believe it will be better for us. Confirm it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that this decision is the most sensible for the moment. You should confirm it&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that with this decision we will have more advantage. Let's do it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I like this decision. Either way the enemy is weaker.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe this is the best strategy to achieve the victory. You should confirm it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with this decision, it is the most sensible. I believe with this decision we will be victorious.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe with this decision we all will be victorious. Confirm it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with you. We need to thank allies in one way or another.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with your decision, we must reduce the damage of defeat. You should confirm this decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I approve this decision, we should invite the enemy leader to visit us. Confirm it and a messenger will be sent.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Supported. I believe everyone will understand this decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with this decision. Confirm it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Very well. I support this decision. You should confirm it immediately.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree that this decision is the right one for the moment.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe this is the best way to know the their opinions.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deverias tentar minimizar a preocupação da população. Pensa bem.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não recomendo que discurses no início do baile, pois podes estragar o mesmo. Caso isso aconteça podes deixar o povo muito preocupado. Recomendo mudar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;O portão é o mais importante. Ele é a entrada para o castelo, tens que impedir que os inimigos entrem. Muda de decisão rapidamente.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a não seres rude agora. Acredito que cruzar os braços não é a melhor decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Recomendo que não aceites, pois pode ser de um inimigo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deverias tentar minimizar a preocupação da população. Pensa bem.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Percebo que este momento não é para piadas. Aconselho a tentar algo mais pessoal e tentar acalma-lo para obter respostas.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Recomendo a que não toques no inimigo, pois ele pode tentar algo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Recomendo que não aceites, pois pode ser de um inimigo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não deverias esconder nada do seu povo, eles vão saber. Pense bem.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Um discurso no final do baile, pode estragar o efeito de felicidade do mesmo. O baile pode amenizar a preocupação gerada por um discurso. Recomendo mudar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -4010,10 +4010,10 @@
       </c>
       <c r="D163" t="str">
         <f>_xlfn.CONCAT(Utt!$A$1,Text!D27,Utt!$C$1)</f>
-        <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;As murálhas são o mais importante. Sem as muralhas o castelo ficará desprotegido contra grandes armas. Mude de decisão rapidamente.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.45">
+        <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;As paredes são o mais importante. Sem as muralhas o castelo ficará desprotegido contra grandes armas. Mude de decisão rapidamente.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a não seres rude agora. Acredito que fingir que não ouviu não é a melhor decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não há a necessidade de recusar a bebida, o serviçal faz parte do nosso povo. E recusando, o povo ficará desapontado&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não deverias esconder nada do seu povo, eles vão saber. Pense bem.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a que não questiones sobre a família, isso pode soar como uma ameaça e, ele ficará mais nervoso. Faça uma piada e descontraia o ambiente.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a teres mais diplomacia, e apertes a mão ao inimigo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não há a necessidade de recusar a bebida, o serviçal faz parte do nosso povo. E recusando, o povo ficará desapontado&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo que esta é a decisão mais correta para lidar com o povo neste momento.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;O baile, é um grande momento e o discurso é realmente necessário para amenizar a preocupação independente quando aconteça.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo que esta região precisa ter prioridade. Confirma rapidamente a tua decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo que esta é melhor decisão para ignorar o inimigo. Confirma-a.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -4189,7 +4189,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Estou de acordo com esta decisão. Tens que confirmar esta decisão para todos saberem.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo que esta é a decisão mais correta para lidar com o povo neste momento.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo que esta decisão irá fazer com que o mensageiro fale. Confirma-a.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo com esta decisão, afinal o inimigo já falou o que tinha para falar.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Estou de acordo com esta decisão. Tens que confirmar esta opção para todos saberem.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should try to minimize the population's concern. Think carefully.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I do not advise the speech at the beginning because it can ruin the ball. If this happens you can leave the people very worried. I recommend changing your decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;The gate is more important. It is the entrance to the castle, you have to prevent the enemies from entering. Change your decision quickly.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise not to be rude at this time. I believe that cross your arms its not the best decision. &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you not to accept, because it can be an enemy.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -4349,7 +4349,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should try to minimize the population's concern. Think carefully.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I realize this moment is not for jokes. I advise you to try something more personal and try to calm him down for answers.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise not to touch the enemy, he can try something.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>186</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you not to accept, because it can be an enemy.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should not hide anything from your people, they will know. Think carefully.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>188</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;A speech at the end can ruin the happy effect of the ball. The ball can soften the concern generated by a speech. I recommend changing your decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;The walls are more important. Without the walls the castle will be unprotected against large weapons. Change your decision quickly.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>190</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise not to be rude at this time. I believe that pretend its not the best decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;There is no need to refuse the drink, it is part of our people. And refusing, the people will get disappointed.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>192</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should not hide anything from your people, they will know. Think carefully.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>193</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you not to question about the family, this may sound like a threat and, he will become more nervous. Make a joke and relax the environment.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>194</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you to have more diplomacy and shake the enemy's hand.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>195</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;There is no need to refuse the drink, it is part of our people. And refusing, the people will get disappointed.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>196</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree that this is the most correct decision to deal with the people at this time.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>197</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;The ball is a great moment and the speech is really necessary to soften the independent concern when it happens.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>198</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree that this region needs to have priority. Confirm your decision quickly.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>199</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree that this is the best decision to ignore the enemy. Confirm it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>200</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with this decision. You have to confirm it for everyone to know.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>201</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree that this is the most correct decision to deal with the people at this time.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>202</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree that this decision will cause the messenger to speak. Confirm it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with this decision, after all the enemy has already spoken what he had to talk about.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>204</v>
       </c>
@@ -4685,97 +4685,97 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with this decision. You have to confirm it for everyone to know.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="B206" s="12"/>
       <c r="C206" s="6"/>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="B207" s="12"/>
       <c r="C207" s="6"/>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
       <c r="B208" s="12"/>
       <c r="C208" s="6"/>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
       <c r="B209" s="12"/>
       <c r="C209" s="6"/>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
       <c r="B210" s="12"/>
       <c r="C210" s="6"/>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
       <c r="B211" s="12"/>
       <c r="C211" s="6"/>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
       <c r="B212" s="12"/>
       <c r="C212" s="6"/>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1"/>
       <c r="B213" s="12"/>
       <c r="C213" s="6"/>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1"/>
       <c r="B214" s="12"/>
       <c r="C214" s="6"/>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
       <c r="B215" s="12"/>
       <c r="C215" s="6"/>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1"/>
       <c r="B216" s="12"/>
       <c r="C216" s="6"/>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1"/>
       <c r="B217" s="12"/>
       <c r="C217" s="6"/>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
       <c r="B218" s="12"/>
       <c r="C218" s="6"/>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1"/>
       <c r="B219" s="12"/>
       <c r="C219" s="6"/>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1"/>
       <c r="B220" s="12"/>
       <c r="C220" s="6"/>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1"/>
       <c r="B221" s="12"/>
       <c r="C221" s="6"/>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1"/>
       <c r="B222" s="12"/>
       <c r="C222" s="6"/>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
       <c r="B223" s="12"/>
       <c r="C223" s="6"/>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
       <c r="B224" s="12"/>
       <c r="C224" s="6"/>
@@ -4809,26 +4809,26 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.73046875" customWidth="1"/>
-    <col min="5" max="5" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.86328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.86328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.86328125" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.265625" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.28515625" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>DP1:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>DP2:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>DP3:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
@@ -5040,7 +5040,7 @@
         <v>DP4:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>58</v>
       </c>
@@ -5090,7 +5090,7 @@
         <v>DP5:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>59</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>DP6:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>60</v>
       </c>
@@ -5190,7 +5190,7 @@
         <v>DP7:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>61</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>DP10:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>62</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>DP11:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="str">
         <f>M1</f>
         <v>DP1:phraseAgainstPref1_PT</v>
@@ -5341,7 +5341,7 @@
         <v>DP12:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="str">
         <f t="shared" ref="B11:B32" si="12">M2</f>
         <v>DP2:phraseAgainstPref1_PT</v>
@@ -5392,7 +5392,7 @@
         <v>DP18:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP3:phraseAgainstPref1_PT</v>
@@ -5443,7 +5443,7 @@
         <v>DP25:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP4:phraseAgainstPref1_PT</v>
@@ -5494,7 +5494,7 @@
         <v>DP26:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP5:phraseAgainstPref1_PT</v>
@@ -5545,7 +5545,7 @@
         <v>DP27:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP6:phraseAgainstPref1_PT</v>
@@ -5596,7 +5596,7 @@
         <v>DP28:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP7:phraseAgainstPref1_PT</v>
@@ -5647,7 +5647,7 @@
         <v>DP29:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP10:phraseAgainstPref1_PT</v>
@@ -5698,7 +5698,7 @@
         <v>DP30:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP11:phraseAgainstPref1_PT</v>
@@ -5749,7 +5749,7 @@
         <v>DP31:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP12:phraseAgainstPref1_PT</v>
@@ -5800,7 +5800,7 @@
         <v>DP32:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP18:phraseAgainstPref1_PT</v>
@@ -5851,7 +5851,7 @@
         <v>DP33:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP25:phraseAgainstPref1_PT</v>
@@ -5902,7 +5902,7 @@
         <v>DP34:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP26:phraseAgainstPref1_PT</v>
@@ -5953,7 +5953,7 @@
         <v>DP35:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP27:phraseAgainstPref1_PT</v>
@@ -6004,7 +6004,7 @@
         <v>DP36:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP28:phraseAgainstPref1_PT</v>
@@ -6013,7 +6013,7 @@
       <c r="H24" s="13"/>
       <c r="J24" s="13"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP29:phraseAgainstPref1_PT</v>
@@ -6064,7 +6064,7 @@
         <v>DG1:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP30:phraseAgainstPref1_PT</v>
@@ -6115,7 +6115,7 @@
         <v>DG2:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP31:phraseAgainstPref1_PT</v>
@@ -6166,7 +6166,7 @@
         <v>DG3:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP32:phraseAgainstPref1_PT</v>
@@ -6217,7 +6217,7 @@
         <v>DG5:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP33:phraseAgainstPref1_PT</v>
@@ -6268,7 +6268,7 @@
         <v>DG9:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP34:phraseAgainstPref1_PT</v>
@@ -6319,7 +6319,7 @@
         <v>DG10:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP35:phraseAgainstPref1_PT</v>
@@ -6370,7 +6370,7 @@
         <v>DG11:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP36:phraseAgainstPref1_PT</v>
@@ -6421,7 +6421,7 @@
         <v>DG14:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="str">
         <f>O1</f>
         <v>DP1:phraseAgainstPref2_PT</v>
@@ -6472,25 +6472,25 @@
         <v>DG19:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="str">
         <f t="shared" ref="B34:B55" si="19">O2</f>
         <v>DP2:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP3:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP4:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP5:phraseAgainstPref2_PT</v>
@@ -6501,7 +6501,7 @@
       <c r="P37" s="14"/>
       <c r="Q37" s="14"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP6:phraseAgainstPref2_PT</v>
@@ -6512,7 +6512,7 @@
       <c r="P38" s="14"/>
       <c r="Q38" s="14"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP7:phraseAgainstPref2_PT</v>
@@ -6523,7 +6523,7 @@
       <c r="P39" s="14"/>
       <c r="Q39" s="14"/>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP10:phraseAgainstPref2_PT</v>
@@ -6534,7 +6534,7 @@
       <c r="P40" s="14"/>
       <c r="Q40" s="14"/>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP11:phraseAgainstPref2_PT</v>
@@ -6545,7 +6545,7 @@
       <c r="P41" s="14"/>
       <c r="Q41" s="14"/>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP12:phraseAgainstPref2_PT</v>
@@ -6556,7 +6556,7 @@
       <c r="P42" s="14"/>
       <c r="Q42" s="14"/>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP18:phraseAgainstPref2_PT</v>
@@ -6567,7 +6567,7 @@
       <c r="P43" s="14"/>
       <c r="Q43" s="14"/>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP25:phraseAgainstPref2_PT</v>
@@ -6578,7 +6578,7 @@
       <c r="P44" s="14"/>
       <c r="Q44" s="14"/>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP26:phraseAgainstPref2_PT</v>
@@ -6589,7 +6589,7 @@
       <c r="P45" s="14"/>
       <c r="Q45" s="14"/>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP27:phraseAgainstPref2_PT</v>
@@ -6600,7 +6600,7 @@
       <c r="P46" s="14"/>
       <c r="Q46" s="14"/>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP28:phraseAgainstPref2_PT</v>
@@ -6611,7 +6611,7 @@
       <c r="P47" s="14"/>
       <c r="Q47" s="14"/>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP29:phraseAgainstPref2_PT</v>
@@ -6622,7 +6622,7 @@
       <c r="P48" s="14"/>
       <c r="Q48" s="14"/>
     </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B49" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP30:phraseAgainstPref2_PT</v>
@@ -6633,7 +6633,7 @@
       <c r="P49" s="14"/>
       <c r="Q49" s="14"/>
     </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP31:phraseAgainstPref2_PT</v>
@@ -6644,7 +6644,7 @@
       <c r="P50" s="14"/>
       <c r="Q50" s="14"/>
     </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP32:phraseAgainstPref2_PT</v>
@@ -6655,7 +6655,7 @@
       <c r="P51" s="14"/>
       <c r="Q51" s="14"/>
     </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B52" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP33:phraseAgainstPref2_PT</v>
@@ -6666,7 +6666,7 @@
       <c r="P52" s="14"/>
       <c r="Q52" s="14"/>
     </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP34:phraseAgainstPref2_PT</v>
@@ -6677,7 +6677,7 @@
       <c r="P53" s="14"/>
       <c r="Q53" s="14"/>
     </row>
-    <row r="54" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP35:phraseAgainstPref2_PT</v>
@@ -6688,7 +6688,7 @@
       <c r="P54" s="14"/>
       <c r="Q54" s="14"/>
     </row>
-    <row r="55" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP36:phraseAgainstPref2_PT</v>
@@ -6699,7 +6699,7 @@
       <c r="P55" s="14"/>
       <c r="Q55" s="14"/>
     </row>
-    <row r="56" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B56" s="8" t="str">
         <f>Q1</f>
         <v>DP1:phraseFavourPref_PT</v>
@@ -6710,7 +6710,7 @@
       <c r="P56" s="14"/>
       <c r="Q56" s="14"/>
     </row>
-    <row r="57" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B57" s="8" t="str">
         <f t="shared" ref="B57:B78" si="20">Q2</f>
         <v>DP2:phraseFavourPref_PT</v>
@@ -6721,7 +6721,7 @@
       <c r="P57" s="14"/>
       <c r="Q57" s="14"/>
     </row>
-    <row r="58" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B58" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP3:phraseFavourPref_PT</v>
@@ -6732,7 +6732,7 @@
       <c r="P58" s="14"/>
       <c r="Q58" s="14"/>
     </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B59" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP4:phraseFavourPref_PT</v>
@@ -6743,7 +6743,7 @@
       <c r="P59" s="14"/>
       <c r="Q59" s="14"/>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B60" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP5:phraseFavourPref_PT</v>
@@ -6754,7 +6754,7 @@
       <c r="P60" s="14"/>
       <c r="Q60" s="14"/>
     </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B61" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP6:phraseFavourPref_PT</v>
@@ -6765,7 +6765,7 @@
       <c r="P61" s="14"/>
       <c r="Q61" s="14"/>
     </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B62" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP7:phraseFavourPref_PT</v>
@@ -6776,7 +6776,7 @@
       <c r="P62" s="14"/>
       <c r="Q62" s="14"/>
     </row>
-    <row r="63" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B63" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP10:phraseFavourPref_PT</v>
@@ -6787,7 +6787,7 @@
       <c r="P63" s="14"/>
       <c r="Q63" s="14"/>
     </row>
-    <row r="64" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B64" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP11:phraseFavourPref_PT</v>
@@ -6798,7 +6798,7 @@
       <c r="P64" s="14"/>
       <c r="Q64" s="14"/>
     </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B65" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP12:phraseFavourPref_PT</v>
@@ -6809,7 +6809,7 @@
       <c r="P65" s="14"/>
       <c r="Q65" s="14"/>
     </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B66" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP18:phraseFavourPref_PT</v>
@@ -6820,7 +6820,7 @@
       <c r="P66" s="14"/>
       <c r="Q66" s="14"/>
     </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B67" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP25:phraseFavourPref_PT</v>
@@ -6831,7 +6831,7 @@
       <c r="P67" s="14"/>
       <c r="Q67" s="14"/>
     </row>
-    <row r="68" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B68" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP26:phraseFavourPref_PT</v>
@@ -6842,7 +6842,7 @@
       <c r="P68" s="14"/>
       <c r="Q68" s="14"/>
     </row>
-    <row r="69" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B69" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP27:phraseFavourPref_PT</v>
@@ -6853,7 +6853,7 @@
       <c r="P69" s="14"/>
       <c r="Q69" s="14"/>
     </row>
-    <row r="70" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B70" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP28:phraseFavourPref_PT</v>
@@ -6864,7 +6864,7 @@
       <c r="P70" s="14"/>
       <c r="Q70" s="14"/>
     </row>
-    <row r="71" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B71" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP29:phraseFavourPref_PT</v>
@@ -6875,7 +6875,7 @@
       <c r="P71" s="14"/>
       <c r="Q71" s="14"/>
     </row>
-    <row r="72" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B72" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP30:phraseFavourPref_PT</v>
@@ -6886,7 +6886,7 @@
       <c r="P72" s="14"/>
       <c r="Q72" s="14"/>
     </row>
-    <row r="73" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B73" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP31:phraseFavourPref_PT</v>
@@ -6897,7 +6897,7 @@
       <c r="P73" s="14"/>
       <c r="Q73" s="14"/>
     </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B74" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP32:phraseFavourPref_PT</v>
@@ -6908,7 +6908,7 @@
       <c r="P74" s="14"/>
       <c r="Q74" s="14"/>
     </row>
-    <row r="75" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B75" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP33:phraseFavourPref_PT</v>
@@ -6919,7 +6919,7 @@
       <c r="P75" s="14"/>
       <c r="Q75" s="14"/>
     </row>
-    <row r="76" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B76" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP34:phraseFavourPref_PT</v>
@@ -6930,7 +6930,7 @@
       <c r="P76" s="14"/>
       <c r="Q76" s="14"/>
     </row>
-    <row r="77" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B77" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP35:phraseFavourPref_PT</v>
@@ -6941,7 +6941,7 @@
       <c r="P77" s="14"/>
       <c r="Q77" s="14"/>
     </row>
-    <row r="78" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B78" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP36:phraseFavourPref_PT</v>
@@ -6952,7 +6952,7 @@
       <c r="P78" s="14"/>
       <c r="Q78" s="14"/>
     </row>
-    <row r="79" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B79" s="8" t="str">
         <f>J1</f>
         <v>DP1:phraseAgainstPref1_EN</v>
@@ -6963,7 +6963,7 @@
       <c r="P79" s="14"/>
       <c r="Q79" s="14"/>
     </row>
-    <row r="80" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B80" s="8" t="str">
         <f t="shared" ref="B80:B101" si="21">J2</f>
         <v>DP2:phraseAgainstPref1_EN</v>
@@ -6974,7 +6974,7 @@
       <c r="P80" s="14"/>
       <c r="Q80" s="14"/>
     </row>
-    <row r="81" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP3:phraseAgainstPref1_EN</v>
@@ -6985,7 +6985,7 @@
       <c r="P81" s="14"/>
       <c r="Q81" s="14"/>
     </row>
-    <row r="82" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B82" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP4:phraseAgainstPref1_EN</v>
@@ -6996,7 +6996,7 @@
       <c r="P82" s="14"/>
       <c r="Q82" s="14"/>
     </row>
-    <row r="83" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B83" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP5:phraseAgainstPref1_EN</v>
@@ -7007,7 +7007,7 @@
       <c r="P83" s="14"/>
       <c r="Q83" s="14"/>
     </row>
-    <row r="84" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="84" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B84" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP6:phraseAgainstPref1_EN</v>
@@ -7018,7 +7018,7 @@
       <c r="P84" s="14"/>
       <c r="Q84" s="14"/>
     </row>
-    <row r="85" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="85" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B85" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP7:phraseAgainstPref1_EN</v>
@@ -7029,7 +7029,7 @@
       <c r="P85" s="14"/>
       <c r="Q85" s="14"/>
     </row>
-    <row r="86" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="86" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B86" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP10:phraseAgainstPref1_EN</v>
@@ -7040,7 +7040,7 @@
       <c r="P86" s="14"/>
       <c r="Q86" s="14"/>
     </row>
-    <row r="87" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="87" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B87" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP11:phraseAgainstPref1_EN</v>
@@ -7051,7 +7051,7 @@
       <c r="P87" s="14"/>
       <c r="Q87" s="14"/>
     </row>
-    <row r="88" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="88" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B88" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP12:phraseAgainstPref1_EN</v>
@@ -7062,7 +7062,7 @@
       <c r="P88" s="14"/>
       <c r="Q88" s="14"/>
     </row>
-    <row r="89" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="89" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B89" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP18:phraseAgainstPref1_EN</v>
@@ -7073,7 +7073,7 @@
       <c r="P89" s="14"/>
       <c r="Q89" s="14"/>
     </row>
-    <row r="90" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B90" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP25:phraseAgainstPref1_EN</v>
@@ -7084,7 +7084,7 @@
       <c r="P90" s="14"/>
       <c r="Q90" s="14"/>
     </row>
-    <row r="91" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="91" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B91" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP26:phraseAgainstPref1_EN</v>
@@ -7095,7 +7095,7 @@
       <c r="P91" s="14"/>
       <c r="Q91" s="14"/>
     </row>
-    <row r="92" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="92" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B92" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP27:phraseAgainstPref1_EN</v>
@@ -7106,7 +7106,7 @@
       <c r="P92" s="14"/>
       <c r="Q92" s="14"/>
     </row>
-    <row r="93" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="93" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B93" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP28:phraseAgainstPref1_EN</v>
@@ -7117,7 +7117,7 @@
       <c r="P93" s="14"/>
       <c r="Q93" s="14"/>
     </row>
-    <row r="94" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="94" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B94" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP29:phraseAgainstPref1_EN</v>
@@ -7128,7 +7128,7 @@
       <c r="P94" s="14"/>
       <c r="Q94" s="14"/>
     </row>
-    <row r="95" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="95" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B95" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP30:phraseAgainstPref1_EN</v>
@@ -7139,7 +7139,7 @@
       <c r="P95" s="14"/>
       <c r="Q95" s="14"/>
     </row>
-    <row r="96" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="96" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B96" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP31:phraseAgainstPref1_EN</v>
@@ -7150,7 +7150,7 @@
       <c r="P96" s="14"/>
       <c r="Q96" s="14"/>
     </row>
-    <row r="97" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="97" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B97" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP32:phraseAgainstPref1_EN</v>
@@ -7161,7 +7161,7 @@
       <c r="P97" s="14"/>
       <c r="Q97" s="14"/>
     </row>
-    <row r="98" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="98" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B98" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP33:phraseAgainstPref1_EN</v>
@@ -7172,7 +7172,7 @@
       <c r="P98" s="14"/>
       <c r="Q98" s="14"/>
     </row>
-    <row r="99" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="99" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP34:phraseAgainstPref1_EN</v>
@@ -7183,7 +7183,7 @@
       <c r="P99" s="14"/>
       <c r="Q99" s="14"/>
     </row>
-    <row r="100" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="100" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B100" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP35:phraseAgainstPref1_EN</v>
@@ -7194,7 +7194,7 @@
       <c r="P100" s="14"/>
       <c r="Q100" s="14"/>
     </row>
-    <row r="101" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="101" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B101" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP36:phraseAgainstPref1_EN</v>
@@ -7205,7 +7205,7 @@
       <c r="P101" s="14"/>
       <c r="Q101" s="14"/>
     </row>
-    <row r="102" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="102" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B102" s="8" t="str">
         <f>H1</f>
         <v>DP1:phraseAgainstPref2_EN</v>
@@ -7216,7 +7216,7 @@
       <c r="P102" s="14"/>
       <c r="Q102" s="14"/>
     </row>
-    <row r="103" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="103" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B103" s="8" t="str">
         <f t="shared" ref="B103:B124" si="22">H2</f>
         <v>DP2:phraseAgainstPref2_EN</v>
@@ -7227,7 +7227,7 @@
       <c r="P103" s="14"/>
       <c r="Q103" s="14"/>
     </row>
-    <row r="104" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="104" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B104" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP3:phraseAgainstPref2_EN</v>
@@ -7238,7 +7238,7 @@
       <c r="P104" s="14"/>
       <c r="Q104" s="14"/>
     </row>
-    <row r="105" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="105" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B105" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP4:phraseAgainstPref2_EN</v>
@@ -7249,7 +7249,7 @@
       <c r="P105" s="14"/>
       <c r="Q105" s="14"/>
     </row>
-    <row r="106" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="106" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B106" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP5:phraseAgainstPref2_EN</v>
@@ -7260,7 +7260,7 @@
       <c r="P106" s="14"/>
       <c r="Q106" s="14"/>
     </row>
-    <row r="107" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="107" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B107" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP6:phraseAgainstPref2_EN</v>
@@ -7271,7 +7271,7 @@
       <c r="P107" s="14"/>
       <c r="Q107" s="14"/>
     </row>
-    <row r="108" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="108" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B108" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP7:phraseAgainstPref2_EN</v>
@@ -7282,7 +7282,7 @@
       <c r="P108" s="14"/>
       <c r="Q108" s="14"/>
     </row>
-    <row r="109" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="109" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B109" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP10:phraseAgainstPref2_EN</v>
@@ -7293,7 +7293,7 @@
       <c r="P109" s="14"/>
       <c r="Q109" s="14"/>
     </row>
-    <row r="110" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="110" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B110" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP11:phraseAgainstPref2_EN</v>
@@ -7304,7 +7304,7 @@
       <c r="P110" s="14"/>
       <c r="Q110" s="14"/>
     </row>
-    <row r="111" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="111" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B111" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP12:phraseAgainstPref2_EN</v>
@@ -7315,7 +7315,7 @@
       <c r="P111" s="14"/>
       <c r="Q111" s="14"/>
     </row>
-    <row r="112" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="112" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B112" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP18:phraseAgainstPref2_EN</v>
@@ -7326,7 +7326,7 @@
       <c r="P112" s="14"/>
       <c r="Q112" s="14"/>
     </row>
-    <row r="113" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="113" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B113" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP25:phraseAgainstPref2_EN</v>
@@ -7337,7 +7337,7 @@
       <c r="P113" s="14"/>
       <c r="Q113" s="14"/>
     </row>
-    <row r="114" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="114" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B114" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP26:phraseAgainstPref2_EN</v>
@@ -7348,7 +7348,7 @@
       <c r="P114" s="14"/>
       <c r="Q114" s="14"/>
     </row>
-    <row r="115" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="115" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B115" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP27:phraseAgainstPref2_EN</v>
@@ -7359,7 +7359,7 @@
       <c r="P115" s="14"/>
       <c r="Q115" s="14"/>
     </row>
-    <row r="116" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="116" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B116" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP28:phraseAgainstPref2_EN</v>
@@ -7370,7 +7370,7 @@
       <c r="P116" s="14"/>
       <c r="Q116" s="14"/>
     </row>
-    <row r="117" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="117" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B117" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP29:phraseAgainstPref2_EN</v>
@@ -7381,7 +7381,7 @@
       <c r="P117" s="14"/>
       <c r="Q117" s="14"/>
     </row>
-    <row r="118" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="118" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B118" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP30:phraseAgainstPref2_EN</v>
@@ -7392,7 +7392,7 @@
       <c r="P118" s="14"/>
       <c r="Q118" s="14"/>
     </row>
-    <row r="119" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="119" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B119" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP31:phraseAgainstPref2_EN</v>
@@ -7403,7 +7403,7 @@
       <c r="P119" s="14"/>
       <c r="Q119" s="14"/>
     </row>
-    <row r="120" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="120" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B120" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP32:phraseAgainstPref2_EN</v>
@@ -7414,7 +7414,7 @@
       <c r="P120" s="14"/>
       <c r="Q120" s="14"/>
     </row>
-    <row r="121" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="121" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B121" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP33:phraseAgainstPref2_EN</v>
@@ -7425,7 +7425,7 @@
       <c r="P121" s="14"/>
       <c r="Q121" s="14"/>
     </row>
-    <row r="122" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="122" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B122" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP34:phraseAgainstPref2_EN</v>
@@ -7436,7 +7436,7 @@
       <c r="P122" s="14"/>
       <c r="Q122" s="14"/>
     </row>
-    <row r="123" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="123" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B123" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP35:phraseAgainstPref2_EN</v>
@@ -7447,7 +7447,7 @@
       <c r="P123" s="14"/>
       <c r="Q123" s="14"/>
     </row>
-    <row r="124" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="124" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B124" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP36:phraseAgainstPref2_EN</v>
@@ -7458,7 +7458,7 @@
       <c r="P124" s="14"/>
       <c r="Q124" s="14"/>
     </row>
-    <row r="125" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="125" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B125" s="8" t="str">
         <f>F1</f>
         <v>DP1:phraseFavourPref_EN</v>
@@ -7469,7 +7469,7 @@
       <c r="P125" s="14"/>
       <c r="Q125" s="14"/>
     </row>
-    <row r="126" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="126" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B126" s="8" t="str">
         <f t="shared" ref="B126:B146" si="23">F2</f>
         <v>DP2:phraseFavourPref_EN</v>
@@ -7480,7 +7480,7 @@
       <c r="P126" s="14"/>
       <c r="Q126" s="14"/>
     </row>
-    <row r="127" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="127" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B127" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP3:phraseFavourPref_EN</v>
@@ -7491,7 +7491,7 @@
       <c r="P127" s="14"/>
       <c r="Q127" s="14"/>
     </row>
-    <row r="128" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="128" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B128" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP4:phraseFavourPref_EN</v>
@@ -7502,7 +7502,7 @@
       <c r="P128" s="14"/>
       <c r="Q128" s="14"/>
     </row>
-    <row r="129" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="129" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B129" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP5:phraseFavourPref_EN</v>
@@ -7513,7 +7513,7 @@
       <c r="P129" s="14"/>
       <c r="Q129" s="14"/>
     </row>
-    <row r="130" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="130" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B130" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP6:phraseFavourPref_EN</v>
@@ -7524,7 +7524,7 @@
       <c r="P130" s="14"/>
       <c r="Q130" s="14"/>
     </row>
-    <row r="131" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="131" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B131" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP7:phraseFavourPref_EN</v>
@@ -7535,7 +7535,7 @@
       <c r="P131" s="14"/>
       <c r="Q131" s="14"/>
     </row>
-    <row r="132" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="132" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B132" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP10:phraseFavourPref_EN</v>
@@ -7546,7 +7546,7 @@
       <c r="P132" s="14"/>
       <c r="Q132" s="14"/>
     </row>
-    <row r="133" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="133" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B133" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP11:phraseFavourPref_EN</v>
@@ -7557,7 +7557,7 @@
       <c r="P133" s="14"/>
       <c r="Q133" s="14"/>
     </row>
-    <row r="134" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="134" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B134" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP12:phraseFavourPref_EN</v>
@@ -7568,7 +7568,7 @@
       <c r="P134" s="14"/>
       <c r="Q134" s="14"/>
     </row>
-    <row r="135" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="135" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B135" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP18:phraseFavourPref_EN</v>
@@ -7579,7 +7579,7 @@
       <c r="P135" s="14"/>
       <c r="Q135" s="14"/>
     </row>
-    <row r="136" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="136" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B136" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP25:phraseFavourPref_EN</v>
@@ -7590,7 +7590,7 @@
       <c r="P136" s="14"/>
       <c r="Q136" s="14"/>
     </row>
-    <row r="137" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="137" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B137" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP26:phraseFavourPref_EN</v>
@@ -7601,7 +7601,7 @@
       <c r="P137" s="14"/>
       <c r="Q137" s="14"/>
     </row>
-    <row r="138" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="138" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B138" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP27:phraseFavourPref_EN</v>
@@ -7612,7 +7612,7 @@
       <c r="P138" s="14"/>
       <c r="Q138" s="14"/>
     </row>
-    <row r="139" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="139" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B139" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP28:phraseFavourPref_EN</v>
@@ -7623,7 +7623,7 @@
       <c r="P139" s="14"/>
       <c r="Q139" s="14"/>
     </row>
-    <row r="140" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="140" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B140" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP29:phraseFavourPref_EN</v>
@@ -7634,7 +7634,7 @@
       <c r="P140" s="14"/>
       <c r="Q140" s="14"/>
     </row>
-    <row r="141" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="141" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B141" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP30:phraseFavourPref_EN</v>
@@ -7645,7 +7645,7 @@
       <c r="P141" s="14"/>
       <c r="Q141" s="14"/>
     </row>
-    <row r="142" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="142" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B142" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP31:phraseFavourPref_EN</v>
@@ -7656,7 +7656,7 @@
       <c r="P142" s="14"/>
       <c r="Q142" s="14"/>
     </row>
-    <row r="143" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="143" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B143" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP32:phraseFavourPref_EN</v>
@@ -7667,7 +7667,7 @@
       <c r="P143" s="14"/>
       <c r="Q143" s="14"/>
     </row>
-    <row r="144" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="144" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B144" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP33:phraseFavourPref_EN</v>
@@ -7678,7 +7678,7 @@
       <c r="P144" s="14"/>
       <c r="Q144" s="14"/>
     </row>
-    <row r="145" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="145" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B145" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP34:phraseFavourPref_EN</v>
@@ -7689,7 +7689,7 @@
       <c r="P145" s="14"/>
       <c r="Q145" s="14"/>
     </row>
-    <row r="146" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="146" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B146" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP35:phraseFavourPref_EN</v>
@@ -7700,7 +7700,7 @@
       <c r="P146" s="14"/>
       <c r="Q146" s="14"/>
     </row>
-    <row r="147" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="147" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B147" s="8" t="str">
         <f>F23</f>
         <v>DP36:phraseFavourPref_EN</v>
@@ -7711,7 +7711,7 @@
       <c r="P147" s="14"/>
       <c r="Q147" s="14"/>
     </row>
-    <row r="148" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="148" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B148" s="8" t="str">
         <f>M25</f>
         <v>DG1:phraseAgainstPref1_PT</v>
@@ -7722,7 +7722,7 @@
       <c r="P148" s="14"/>
       <c r="Q148" s="14"/>
     </row>
-    <row r="149" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="149" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B149" s="8" t="str">
         <f t="shared" ref="B149:B156" si="24">M26</f>
         <v>DG2:phraseAgainstPref1_PT</v>
@@ -7733,7 +7733,7 @@
       <c r="P149" s="14"/>
       <c r="Q149" s="14"/>
     </row>
-    <row r="150" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="150" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B150" s="8" t="str">
         <f t="shared" si="24"/>
         <v>DG3:phraseAgainstPref1_PT</v>
@@ -7744,7 +7744,7 @@
       <c r="P150" s="14"/>
       <c r="Q150" s="14"/>
     </row>
-    <row r="151" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="151" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B151" s="8" t="str">
         <f t="shared" si="24"/>
         <v>DG5:phraseAgainstPref1_PT</v>
@@ -7755,7 +7755,7 @@
       <c r="P151" s="14"/>
       <c r="Q151" s="14"/>
     </row>
-    <row r="152" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="152" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B152" s="8" t="str">
         <f t="shared" si="24"/>
         <v>DG9:phraseAgainstPref1_PT</v>
@@ -7766,7 +7766,7 @@
       <c r="P152" s="14"/>
       <c r="Q152" s="14"/>
     </row>
-    <row r="153" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="153" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B153" s="8" t="str">
         <f t="shared" si="24"/>
         <v>DG10:phraseAgainstPref1_PT</v>
@@ -7777,7 +7777,7 @@
       <c r="P153" s="14"/>
       <c r="Q153" s="14"/>
     </row>
-    <row r="154" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="154" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B154" s="8" t="str">
         <f t="shared" si="24"/>
         <v>DG11:phraseAgainstPref1_PT</v>
@@ -7788,7 +7788,7 @@
       <c r="P154" s="14"/>
       <c r="Q154" s="14"/>
     </row>
-    <row r="155" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="155" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B155" s="8" t="str">
         <f t="shared" si="24"/>
         <v>DG14:phraseAgainstPref1_PT</v>
@@ -7799,7 +7799,7 @@
       <c r="P155" s="14"/>
       <c r="Q155" s="14"/>
     </row>
-    <row r="156" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="156" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B156" s="8" t="str">
         <f t="shared" si="24"/>
         <v>DG19:phraseAgainstPref1_PT</v>
@@ -7810,7 +7810,7 @@
       <c r="P156" s="14"/>
       <c r="Q156" s="14"/>
     </row>
-    <row r="157" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="157" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B157" s="8" t="str">
         <f>O25</f>
         <v>DG1:phraseAgainstPref2_PT</v>
@@ -7821,7 +7821,7 @@
       <c r="P157" s="14"/>
       <c r="Q157" s="14"/>
     </row>
-    <row r="158" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="158" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B158" s="8" t="str">
         <f t="shared" ref="B158:B165" si="25">O26</f>
         <v>DG2:phraseAgainstPref2_PT</v>
@@ -7832,259 +7832,259 @@
       <c r="P158" s="14"/>
       <c r="Q158" s="14"/>
     </row>
-    <row r="159" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="159" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B159" s="8" t="str">
         <f t="shared" si="25"/>
         <v>DG3:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="160" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="160" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B160" s="8" t="str">
         <f t="shared" si="25"/>
         <v>DG5:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="161" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B161" s="8" t="str">
         <f t="shared" si="25"/>
         <v>DG9:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="162" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B162" s="8" t="str">
         <f t="shared" si="25"/>
         <v>DG10:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="163" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B163" s="8" t="str">
         <f t="shared" si="25"/>
         <v>DG11:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="164" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B164" s="8" t="str">
         <f t="shared" si="25"/>
         <v>DG14:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="165" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B165" s="8" t="str">
         <f t="shared" si="25"/>
         <v>DG19:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" s="8" t="str">
         <f>Q25</f>
         <v>DG1:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" s="8" t="str">
         <f t="shared" ref="B167:B174" si="26">Q26</f>
         <v>DG2:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B168" s="8" t="str">
         <f t="shared" si="26"/>
         <v>DG3:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B169" s="8" t="str">
         <f t="shared" si="26"/>
         <v>DG5:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B170" s="8" t="str">
         <f t="shared" si="26"/>
         <v>DG9:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B171" s="8" t="str">
         <f t="shared" si="26"/>
         <v>DG10:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" s="8" t="str">
         <f t="shared" si="26"/>
         <v>DG11:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" s="8" t="str">
         <f t="shared" si="26"/>
         <v>DG14:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B174" s="8" t="str">
         <f t="shared" si="26"/>
         <v>DG19:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="175" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B175" s="8" t="str">
         <f>J25</f>
         <v>DG1:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="176" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B176" s="8" t="str">
         <f t="shared" ref="B176:B183" si="27">J26</f>
         <v>DG2:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="177" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B177" s="8" t="str">
         <f t="shared" si="27"/>
         <v>DG3:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="178" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B178" s="8" t="str">
         <f t="shared" si="27"/>
         <v>DG5:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="179" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B179" s="8" t="str">
         <f t="shared" si="27"/>
         <v>DG9:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="180" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B180" s="8" t="str">
         <f t="shared" si="27"/>
         <v>DG10:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="181" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B181" s="8" t="str">
         <f t="shared" si="27"/>
         <v>DG11:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="182" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B182" s="8" t="str">
         <f t="shared" si="27"/>
         <v>DG14:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="183" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B183" s="8" t="str">
         <f t="shared" si="27"/>
         <v>DG19:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="184" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B184" s="8" t="str">
         <f>H25</f>
         <v>DG1:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="185" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B185" s="8" t="str">
         <f t="shared" ref="B185:B192" si="28">H26</f>
         <v>DG2:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="186" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B186" s="8" t="str">
         <f t="shared" si="28"/>
         <v>DG3:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="187" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B187" s="8" t="str">
         <f t="shared" si="28"/>
         <v>DG5:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="188" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B188" s="8" t="str">
         <f t="shared" si="28"/>
         <v>DG9:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="189" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B189" s="8" t="str">
         <f t="shared" si="28"/>
         <v>DG10:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="190" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B190" s="8" t="str">
         <f t="shared" si="28"/>
         <v>DG11:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="191" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B191" s="8" t="str">
         <f t="shared" si="28"/>
         <v>DG14:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="192" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B192" s="8" t="str">
         <f t="shared" si="28"/>
         <v>DG19:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B193" s="8" t="str">
         <f>F25</f>
         <v>DG1:phraseFavourPref_EN</v>
       </c>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B194" s="8" t="str">
         <f t="shared" ref="B194:B200" si="29">F26</f>
         <v>DG2:phraseFavourPref_EN</v>
       </c>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B195" s="8" t="str">
         <f t="shared" si="29"/>
         <v>DG3:phraseFavourPref_EN</v>
       </c>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B196" s="8" t="str">
         <f t="shared" si="29"/>
         <v>DG5:phraseFavourPref_EN</v>
       </c>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B197" s="8" t="str">
         <f t="shared" si="29"/>
         <v>DG9:phraseFavourPref_EN</v>
       </c>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="198" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B198" s="8" t="str">
         <f t="shared" si="29"/>
         <v>DG10:phraseFavourPref_EN</v>
       </c>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="199" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B199" s="8" t="str">
         <f t="shared" si="29"/>
         <v>DG11:phraseFavourPref_EN</v>
       </c>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="200" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B200" s="8" t="str">
         <f t="shared" si="29"/>
         <v>DG14:phraseFavourPref_EN</v>
       </c>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="201" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B201" s="8" t="str">
         <f>F33</f>
         <v>DG19:phraseFavourPref_EN</v>
@@ -8099,23 +8099,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7405BC36-7328-40C6-8088-275F0F9C1320}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="71.59765625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="78" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.86328125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="76.86328125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="69.265625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="55.1328125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="60.85546875" style="16" customWidth="1"/>
+    <col min="6" max="6" width="76.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="69.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="55.140625" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -8141,7 +8141,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -8149,10 +8149,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>101</v>
@@ -8167,7 +8167,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -8175,7 +8175,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>102</v>
@@ -8193,7 +8193,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -8219,7 +8219,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -8227,7 +8227,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>131</v>
@@ -8245,7 +8245,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -8259,7 +8259,7 @@
         <v>45</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>112</v>
@@ -8271,7 +8271,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -8297,7 +8297,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -8323,7 +8323,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -8349,7 +8349,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -8357,7 +8357,7 @@
         <v>21</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>134</v>
@@ -8375,7 +8375,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -8401,7 +8401,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -8415,7 +8415,7 @@
         <v>146</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>147</v>
@@ -8427,7 +8427,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -8453,7 +8453,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -8479,7 +8479,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -8493,7 +8493,7 @@
         <v>163</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>161</v>
@@ -8505,7 +8505,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -8513,7 +8513,7 @@
         <v>27</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>165</v>
@@ -8531,7 +8531,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="15" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>15</v>
       </c>
@@ -8539,7 +8539,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>173</v>
@@ -8557,7 +8557,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -8565,7 +8565,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>175</v>
@@ -8583,7 +8583,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -8609,7 +8609,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -8617,7 +8617,7 @@
         <v>31</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>187</v>
@@ -8635,7 +8635,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -8643,13 +8643,13 @@
         <v>32</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>189</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>191</v>
@@ -8661,7 +8661,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -8687,7 +8687,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -8713,7 +8713,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -8721,7 +8721,7 @@
         <v>35</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D24" s="16" t="s">
         <v>203</v>
@@ -8739,7 +8739,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -8747,7 +8747,7 @@
         <v>43</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D25" s="16" t="s">
         <v>208</v>
@@ -8765,7 +8765,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -8791,7 +8791,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -8799,25 +8799,25 @@
         <v>46</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D27" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="F27" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="E27" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="F27" s="16" t="s">
+      <c r="G27" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="H27" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="H27" s="16" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -8825,25 +8825,25 @@
         <v>47</v>
       </c>
       <c r="C28" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="D28" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="E28" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="F28" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="E28" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="F28" s="16" t="s">
+      <c r="G28" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="G28" s="16" t="s">
+      <c r="H28" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="H28" s="16" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -8854,22 +8854,22 @@
         <v>64</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F29" s="16" t="s">
         <v>85</v>
       </c>
       <c r="G29" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="H29" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="H29" s="16" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -8877,7 +8877,7 @@
         <v>49</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D30" s="16" t="s">
         <v>208</v>
@@ -8895,7 +8895,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -8903,25 +8903,25 @@
         <v>50</v>
       </c>
       <c r="C31" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="F31" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="G31" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="H31" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="E31" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>231</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -8947,7 +8947,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -8958,19 +8958,19 @@
         <v>64</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>85</v>
       </c>
       <c r="G33" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="H33" s="16" t="s">
         <v>227</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -8990,13 +8990,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="77" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Changed condtion for shame robot
</commit_message>
<xml_diff>
--- a/SOP/Utterances/phrasesAgainstPositive.xlsx
+++ b/SOP/Utterances/phrasesAgainstPositive.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marie\Desktop\Git\Storytelling_SR\SOP\Utterances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria José Ferreira\Desktop\GitStorytelling\SOP\Utterances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2898A09F-B112-4E7E-AE2A-395A3ED8BF48}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17E1D8E-9934-47C1-860B-BDBB72CDD430}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11415" activeTab="2" xr2:uid="{44FFEBE6-F1D8-41FA-8CF8-D767FF193A3D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11415" xr2:uid="{44FFEBE6-F1D8-41FA-8CF8-D767FF193A3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Utterances" sheetId="3" r:id="rId1"/>
@@ -476,9 +476,6 @@
     <t>I approve this decision, I believe it will be better for us. Confirm it.</t>
   </si>
   <si>
-    <t>Recomendo a agir rapidamente, pois precisamos de mais militares com urgência.</t>
-  </si>
-  <si>
     <t>Deves pensar melhor nesta intenção, pois a população pode ser muito afectada com esta decisão.</t>
   </si>
   <si>
@@ -812,9 +809,6 @@
     <t>Estou de acordo com esta decisão. Tens que confirmar esta opção para todos saberem.</t>
   </si>
   <si>
-    <t>As paredes são o mais importante. Sem as muralhas o castelo ficará desprotegido contra grandes armas. Mude de decisão rapidamente.</t>
-  </si>
-  <si>
     <t>Acredito que com esta decisão os aliados seremos todos vitóriosos. Deves confirmá-la.</t>
   </si>
   <si>
@@ -825,6 +819,12 @@
   </si>
   <si>
     <t>Acredito que esta é a melhor estratégia para alcançar a vitória. Deves confirmá-la.</t>
+  </si>
+  <si>
+    <t>Recomendo a agir rapidamente, pois precisamos de mais militares com urgência. Mande treinar mais militares. Escolha a outra decisão.</t>
+  </si>
+  <si>
+    <t>As paredes são o mais importante. Sem as paredes do castelo ficará desprotegido contra grandes armas. Mude de decisão rapidamente.</t>
   </si>
 </sst>
 </file>
@@ -1417,19 +1417,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC699C3-7B7D-494D-9389-830F8CDC6B9F}">
   <dimension ref="A1:F224"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="D106" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="7.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.265625" customWidth="1"/>
+    <col min="3" max="3" width="15.1328125" customWidth="1"/>
     <col min="4" max="4" width="219" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1445,7 +1445,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que irás ficar muito espouhsto. Muda de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a não fazer um baile neste momento, e sim a preparar-nos para uma batalha. Escolhe a outra opção.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que ao falares primeiro, podes influenciar os teus conselheiros. Deverias mudar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não deverias te expôr tanto, acho que deverias te retirar do baile. Pensa melhor e muda de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho que converses apenas com os nossos aliados mais antigos.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não te aconselho a deixar que alguém desconhecido entre. Isso é muito perigoso.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Este não é o momento de intérahgir com o adversário. Deverias mudar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho que solicites explicações imediatamente. Quanto mais cedo melhor para o país se preparar.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deixe o falar enquanto tentamos perceber melhor qual a tática dele. Deste modo, as defesas poderão ser preparadas melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1770,10 +1770,10 @@
       </c>
       <c r="D23" t="str">
         <f>_xlfn.CONCAT(Utt!$A$1,Text!C11,Utt!$C$1)</f>
-        <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Recomendo a agir rapidamente, pois precisamos de mais militares com urgência.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Recomendo a agir rapidamente, pois precisamos de mais militares com urgência. Mande treinar mais militares. Escolha a outra decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;A minha intuição diz-me que não há tempo para defender a rua principal. Com esta decisão, iremos perder muitos militares desnecessariamente.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que o mensageiro transmitiu a informação correta. Tens que demonstrar confiança no teu povo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a aproveitar esse tempo para enviar um batalhão de soldados para o ataque e acabar com o inimigo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a enviar uma tropa de soldados rapidamente para garantir a vitória e não deixar os aliados esperando. Pois, eles podem ir embora.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Com apenas metade dos soldados não acho que seremos vitoriósos. Acredito que os aliados não terão força suficiente para derrotar o inimigo. Pensa melhor e, muda de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a não sair da protéção da cidade por enquanto. Ainda é muito arriscado ir ao campo de batalha, podemos ser surpreendidos. Pensa melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não deves te expor ao inimigo desta forma. Além disso, fazer o primeiro contacto indica fraqueza. Pensa melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que deverias ser mais diplomático. Além disso, agradecer o convite é um sinal de educação.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Recomendo que mantenhas a tua liderança e jámais te rendas. Deverias mudar de decisão e mostrar a tua força.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acho que não deves mudar de opinião, pois isso demonstra fraquesa. Pensa melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que há várias maneiras para bloquear o acesso, devias pensar melhore trocar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;O sentimento de patriotismo é importante para incentivar o povo. Deverias mudar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não deves interagir com todos os conselheiros apenas um deve falar. Falar com todos vais ficar muito espouhsto, pode ser perigoso. Pensa melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que deverias falar em público, pois o teu povo precisa saber o que se passa. Muda de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a que organizes um baile para o teu povo ficar mais unido. Escolha a outra opção.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que deverias expressar primeiro a tua opinião. Deverias mudar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que deverias falar com todos no baile para mostrar que estás tranquilo com a situação. Não saia agora, mude de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que conversar com novos aliados trará novas ideias.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho que coñeças o mensageiro. Tens que ver a face do inimigo para conseguir vence-lo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deves tentar ganhar a confiança do adversário convidando-o. Deverias mudar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deverias ser mais gentil, e esperar que o adversário termine de falar. Ele não gosta de ser interrompido, sinto que isso pode apressar a batalha.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deves fazer o adversário parar de falar imediatamente. Acredito que ele quer descobrir algo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deves pensar melhor nesta intenção, pois a população pode ser muito afectada com esta decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a enviar imediatamente soldados para defender a rua. Com esta decisão, o castelo será tomado com maior facilidade pelo inimigo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Sinto que o inimigo não perdeu tanta força como informou o mensageiro. Pouco provável que o mensageiro conseguiria ter a informação correcta em um campo de batalha.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que deves pensar no nosso exército e deixá-lo descansar. Assim, novas estratégias de combate podem ser criadas sem muitas baixas.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Cuidado, se enviares as tropas podemos ficar sem soldados suficientes para nos proteger.  Devemos ter certeza que são aliados, pois podem ser inimigos.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Assim ficaremos fracos e desprutegidos. Acredito que os aliados podem conseguir derrotar o inimigo com metade dos nossos soldados e, ao mesmo tempo, estaremos protegidos. Pense melhor e, mude de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a ires pessoalmente e congratulá-lo pela vitória. Desse modo, mostrarás a todos que não tens medo de nada e de ninguém. Deverias pensar melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deves chamar o líder inimigo. Além disso, chamando ele indicas que ainda és forte. Pense melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que não deves mostrar diplomacia para com o inimigo. Além disso, o inimigo deve entender que ficamos indignados com a ameaça.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Devias negociar, pois o teu povo depende de ti. Deverias mudar de decisão e mostrar que se importas com o povo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que deves mudar de decisão, pois agora deves ter certeza da decisão. Pense melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que agora não há mais nada a fazer para defender o acesso. Estamos perdendo tempo ao pensar em novas ideias.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Agora não precisamos de símbolos, mas sim de ações. Deverias mudar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deverias saber a opinião de cada um dos membros do conselho. Assim todos vão se sentir importantes. Pense melhor.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Esta é a melhor decisão a ser tomada, pois eles precisam saber primeiro. Confirme esta decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Eu gosto desta decisão, pois, é a melhor forma de estar pronto para uma batalha. Confirme-a.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Mantém essa decisão. Todos terão a sua vez de falar.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Estou de acordo com esta decisão. Acredito ser o melhor pra todos.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Entendo o teu ponto de vista e concordo. Aliados são bem vindos neste momento.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que tomastes a melhor decisão para este momento. A outra decisão irá gerar muitos problemas.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que esta decisão é a mais segura para o nosso povo. Confirme-a.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo com esta decisão. Assim, saberemos os motivos no momento ideal.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aprovo esta decisão, acredito que assim será melhor para o povo. Confirme-a.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que esta decisão é a mais sensata para o momento. Deves confirmá-la.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que com esta decisão teremos mais vantagem. Vamos a isto.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Eu gosto desta decisão. De qualquer forma o inimigo está mais fraco.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que esta é a melhor estratégia para alcançar a vitória. Deves confirmá-la.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo com esta decisão, é a mais sensata. Acredito que com isto caminhamos para a vitória.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que com esta decisão os aliados seremos todos vitóriosos. Deves confirmá-la.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo contigo. Precisamos agradecer aos aliados de uma forma ou de outra.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo com a tua decisão, devemos diminuir o estrago da derrota. Deves confirmar esta decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aprovo esta decisão, devemos convidar o líder inimigo para nos visitar. Confirme e um mensageiro será enviado.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Apoiado. Acredito que todos irão entender esta decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo com esta decisão. Confirma-a.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Muito bem, apóio esta decisão. Deverias confirmá-la imediatamente.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo que esta decisão é a mais correta para o momento.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Acredito que esta é a melhor forma de saber a opinião deles.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I think you will be very exposed. Change your decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise that this is not the time for a ball, but to prepare for a battle. Chose the other option.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that by speaking first you can influence your counselors.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should not expose yourself so much and you should withdraw from the ball. Think better, and change your decision. &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advice you just talk to our old allies.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I do not advise anyone unknown to come in. This is very dangerous.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;This is not the time to interact with the enemy. You should change the decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you to request explanations immediately. The sooner the better for the country to prepare.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Let him talk as we try to better understand his tactics. In this way, defenses can be better prepared.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Recommend to act quickly we need more military urgently.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;My intuition says there is no time to defend the main access. With this decision, we will lose many soldiers unnecessarily.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe the messenger has passed on the correct information. You have to show confidence in your people.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you to send a troop to the attack and finishing the enemy.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you to send a troop of soldiers quickly to ensure the victory and not leave the allies waiting. Because, they can leave.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;With only half the soldiers I do not think we will be victorious. I believe that the allies will not have enough strength to defeat the enemy. Think better, and change your mind.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you not to leave the protections of the city yet. It is still very risky to go to the battlefield, we may be surprised. Think better.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should not expose yourself to the enemy in this way. Also, making the first contact indicates weakness. Think better.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I think you should be more diplomatic. Also, thanking the invitation is a sign of education.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I recommend that you should be a leader and never surrender. You should change your mind and show your strength.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I do not think you should change your mind, because it shows weakness. You should think better.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that there are several ideas to block the accesses, you should think better and change your decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;The feeling of patriotism is important to encourage the people. You should change your decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should not interact with everyone on the council just one should talk. Talking to everyone will be very exposed, it can be dangerous. Think better.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that you should to speech to the public, they need to know. Change your decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -3117,7 +3117,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you to organize the ball for the people to be more united.  Chose the other option.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that you should speak first of all to know your opinion.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I think you should talk to everyone at the ball to show peace. Do not leave now, change your decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that talking to new allies will bring new ideas.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you to meet this person. You have to see the enemy's face to defeat him.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -3197,7 +3197,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should try to gain the confidence of the enemy by inviting him. You should change the decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should be kinder and wait for the enemy to finish talking. He does not like being interrupted, I feel that this can hasten the battle.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should immediately make him stop talking. I think he wants to find out something.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should think better about this intention because the population can be very affected whit this decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you to immediately send soldiers to defend access. With this decision, the castle will be taken more easily by the enemy.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I feel that the enemy has not lost as much force as the messenger informs. Unlikely the messenger would get the correct information on a battlefield.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I think you should think about our army and let them rest. Thus, new combat strategies can be created without many casualties.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Be careful, if you send the troops, we can run out of enough soldiers to protect us. We must be sure that allies, they can be enemies.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;That way we'll be weak and out of touch. I believe that the Allies can successfully defeat the enemy with half of our soldiers, and at the same time we will be protected. Think better, and change your mind.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you to go personally and congratulate them for the victory. In this way, you will show to everyone that you are not afraid of anything and nobody. You should think better.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should call the enemy leader. Also, calling him indicates that you're still strong. Think better.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I do not think you should show diplomacy to the enemy. In addition, the enemy must understand that we are outraged by the threat.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should trade, because your people depend on you. You should change your mind and show that you care about the people.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that you must change your decision, because now you are certain of the decision. You should think better.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that there is no longer any way to defend the access. We are wasting time thinking about new ideas.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -3437,7 +3437,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;We do not need symbols, but actions. You should change your decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should know the opinion of each one of the council. So everyone will feel important. Think better.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;This is the best decision to be taken, because they need to know first.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I like this decision, because it is the best way to be ready for a battle. Confirm it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Keep that decision. Everyone will have their turn to speak.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with this decision. I believe that is the best for all.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -3533,7 +3533,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I understand your point of view and agree with it. Allies are welcome at this time.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that you have made the best decision for this moment. The other decision will generate many problems.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that this decision is the safest for our people. Confirm it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with this decision. In this way, we will know the motives at the ideal moment.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I approve this decision, I believe it will be better for us. Confirm it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that this decision is the most sensible for the moment. You should confirm it&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe that with this decision we will have more advantage. Let's do it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I like this decision. Either way the enemy is weaker.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe this is the best strategy to achieve the victory. You should confirm it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with this decision, it is the most sensible. I believe with this decision we will be victorious.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe with this decision we all will be victorious. Confirm it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with you. We need to thank allies in one way or another.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with your decision, we must reduce the damage of defeat. You should confirm this decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I approve this decision, we should invite the enemy leader to visit us. Confirm it and a messenger will be sent.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Supported. I believe everyone will understand this decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with this decision. Confirm it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Very well. I support this decision. You should confirm it immediately.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree that this decision is the right one for the moment.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I believe this is the best way to know the their opinions.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deverias tentar minimizar a preocupação da população. Pensa bem.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não recomendo que discurses no início do baile, pois podes estragar o mesmo. Caso isso aconteça podes deixar o povo muito preocupado. Recomendo mudar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;O portão é o mais importante. Ele é a entrada para o castelo, tens que impedir que os inimigos entrem. Muda de decisão rapidamente.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a não seres rude agora. Acredito que cruzar os braços não é a melhor decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Recomendo que não aceites, pois pode ser de um inimigo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Deverias tentar minimizar a preocupação da população. Pensa bem.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Percebo que este momento não é para piadas. Aconselho a tentar algo mais pessoal e tentar acalma-lo para obter respostas.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Recomendo a que não toques no inimigo, pois ele pode tentar algo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Recomendo que não aceites, pois pode ser de um inimigo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não deverias esconder nada do seu povo, eles vão saber. Pense bem.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Um discurso no final do baile, pode estragar o efeito de felicidade do mesmo. O baile pode amenizar a preocupação gerada por um discurso. Recomendo mudar de decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -4010,10 +4010,10 @@
       </c>
       <c r="D163" t="str">
         <f>_xlfn.CONCAT(Utt!$A$1,Text!D27,Utt!$C$1)</f>
-        <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;As paredes são o mais importante. Sem as muralhas o castelo ficará desprotegido contra grandes armas. Mude de decisão rapidamente.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+        <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;As paredes são o mais importante. Sem as paredes do castelo ficará desprotegido contra grandes armas. Mude de decisão rapidamente.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a não seres rude agora. Acredito que fingir que não ouviu não é a melhor decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não há a necessidade de recusar a bebida, o serviçal faz parte do nosso povo. E recusando, o povo ficará desapontado&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não deverias esconder nada do seu povo, eles vão saber. Pense bem.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a que não questiones sobre a família, isso pode soar como uma ameaça e, ele ficará mais nervoso. Faça uma piada e descontraia o ambiente.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Aconselho a teres mais diplomacia, e apertes a mão ao inimigo.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -4109,7 +4109,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Não há a necessidade de recusar a bebida, o serviçal faz parte do nosso povo. E recusando, o povo ficará desapontado&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo que esta é a decisão mais correta para lidar com o povo neste momento.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;O baile, é um grande momento e o discurso é realmente necessário para amenizar a preocupação independente quando aconteça.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo que esta região precisa ter prioridade. Confirma rapidamente a tua decisão.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo que esta é melhor decisão para ignorar o inimigo. Confirma-a.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -4189,7 +4189,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Estou de acordo com esta decisão. Tens que confirmar esta decisão para todos saberem.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo que esta é a decisão mais correta para lidar com o povo neste momento.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo que esta decisão irá fazer com que o mensageiro fale. Confirma-a.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Concordo com esta decisão, afinal o inimigo já falou o que tinha para falar.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;Estou de acordo com esta decisão. Tens que confirmar esta opção para todos saberem.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should try to minimize the population's concern. Think carefully.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I do not advise the speech at the beginning because it can ruin the ball. If this happens you can leave the people very worried. I recommend changing your decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;The gate is more important. It is the entrance to the castle, you have to prevent the enemies from entering. Change your decision quickly.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -4317,7 +4317,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise not to be rude at this time. I believe that cross your arms its not the best decision. &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you not to accept, because it can be an enemy.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -4349,7 +4349,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should try to minimize the population's concern. Think carefully.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I realize this moment is not for jokes. I advise you to try something more personal and try to calm him down for answers.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise not to touch the enemy, he can try something.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A187" s="1">
         <v>186</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you not to accept, because it can be an enemy.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should not hide anything from your people, they will know. Think carefully.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A189" s="1">
         <v>188</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;A speech at the end can ruin the happy effect of the ball. The ball can soften the concern generated by a speech. I recommend changing your decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;The walls are more important. Without the walls the castle will be unprotected against large weapons. Change your decision quickly.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A191" s="1">
         <v>190</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise not to be rude at this time. I believe that pretend its not the best decision.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;There is no need to refuse the drink, it is part of our people. And refusing, the people will get disappointed.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A193" s="1">
         <v>192</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;You should not hide anything from your people, they will know. Think carefully.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A194" s="1">
         <v>193</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you not to question about the family, this may sound like a threat and, he will become more nervous. Make a joke and relax the environment.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A195" s="1">
         <v>194</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I advise you to have more diplomacy and shake the enemy's hand.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A196" s="1">
         <v>195</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;There is no need to refuse the drink, it is part of our people. And refusing, the people will get disappointed.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A197" s="1">
         <v>196</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree that this is the most correct decision to deal with the people at this time.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A198" s="1">
         <v>197</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;The ball is a great moment and the speech is really necessary to soften the independent concern when it happens.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A199" s="1">
         <v>198</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree that this region needs to have priority. Confirm your decision quickly.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A200" s="1">
         <v>199</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree that this is the best decision to ignore the enemy. Confirm it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A201" s="1">
         <v>200</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with this decision. You have to confirm it for everyone to know.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A202" s="1">
         <v>201</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree that this is the most correct decision to deal with the people at this time.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A203" s="1">
         <v>202</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree that this decision will cause the messenger to speak. Confirm it.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with this decision, after all the enemy has already spoken what he had to talk about.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A205" s="1">
         <v>204</v>
       </c>
@@ -4685,97 +4685,97 @@
         <v>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt;&lt;Gaze(person3)&gt;I agree with this decision. You have to confirm it for everyone to know.&lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A206" s="1"/>
       <c r="B206" s="12"/>
       <c r="C206" s="6"/>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A207" s="1"/>
       <c r="B207" s="12"/>
       <c r="C207" s="6"/>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A208" s="1"/>
       <c r="B208" s="12"/>
       <c r="C208" s="6"/>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A209" s="1"/>
       <c r="B209" s="12"/>
       <c r="C209" s="6"/>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A210" s="1"/>
       <c r="B210" s="12"/>
       <c r="C210" s="6"/>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A211" s="1"/>
       <c r="B211" s="12"/>
       <c r="C211" s="6"/>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A212" s="1"/>
       <c r="B212" s="12"/>
       <c r="C212" s="6"/>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A213" s="1"/>
       <c r="B213" s="12"/>
       <c r="C213" s="6"/>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A214" s="1"/>
       <c r="B214" s="12"/>
       <c r="C214" s="6"/>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A215" s="1"/>
       <c r="B215" s="12"/>
       <c r="C215" s="6"/>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A216" s="1"/>
       <c r="B216" s="12"/>
       <c r="C216" s="6"/>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A217" s="1"/>
       <c r="B217" s="12"/>
       <c r="C217" s="6"/>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A218" s="1"/>
       <c r="B218" s="12"/>
       <c r="C218" s="6"/>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A219" s="1"/>
       <c r="B219" s="12"/>
       <c r="C219" s="6"/>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A220" s="1"/>
       <c r="B220" s="12"/>
       <c r="C220" s="6"/>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A221" s="1"/>
       <c r="B221" s="12"/>
       <c r="C221" s="6"/>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A222" s="1"/>
       <c r="B222" s="12"/>
       <c r="C222" s="6"/>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A223" s="1"/>
       <c r="B223" s="12"/>
       <c r="C223" s="6"/>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A224" s="1"/>
       <c r="B224" s="12"/>
       <c r="C224" s="6"/>
@@ -4809,26 +4809,26 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.73046875" customWidth="1"/>
+    <col min="5" max="5" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.1328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.1328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.86328125" style="13" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.86328125" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.265625" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>DP1:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>DP2:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>DP3:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
@@ -5040,7 +5040,7 @@
         <v>DP4:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B5" s="7" t="s">
         <v>58</v>
       </c>
@@ -5090,7 +5090,7 @@
         <v>DP5:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B6" s="7" t="s">
         <v>59</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>DP6:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B7" s="7" t="s">
         <v>60</v>
       </c>
@@ -5190,7 +5190,7 @@
         <v>DP7:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B8" s="7" t="s">
         <v>61</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>DP10:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B9" s="7" t="s">
         <v>62</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>DP11:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B10" s="8" t="str">
         <f>M1</f>
         <v>DP1:phraseAgainstPref1_PT</v>
@@ -5341,7 +5341,7 @@
         <v>DP12:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B11" s="8" t="str">
         <f t="shared" ref="B11:B32" si="12">M2</f>
         <v>DP2:phraseAgainstPref1_PT</v>
@@ -5392,7 +5392,7 @@
         <v>DP18:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B12" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP3:phraseAgainstPref1_PT</v>
@@ -5443,7 +5443,7 @@
         <v>DP25:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP4:phraseAgainstPref1_PT</v>
@@ -5494,7 +5494,7 @@
         <v>DP26:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B14" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP5:phraseAgainstPref1_PT</v>
@@ -5545,7 +5545,7 @@
         <v>DP27:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B15" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP6:phraseAgainstPref1_PT</v>
@@ -5596,7 +5596,7 @@
         <v>DP28:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B16" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP7:phraseAgainstPref1_PT</v>
@@ -5647,7 +5647,7 @@
         <v>DP29:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="17" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B17" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP10:phraseAgainstPref1_PT</v>
@@ -5698,7 +5698,7 @@
         <v>DP30:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="18" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B18" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP11:phraseAgainstPref1_PT</v>
@@ -5749,7 +5749,7 @@
         <v>DP31:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="19" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B19" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP12:phraseAgainstPref1_PT</v>
@@ -5800,7 +5800,7 @@
         <v>DP32:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="20" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B20" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP18:phraseAgainstPref1_PT</v>
@@ -5851,7 +5851,7 @@
         <v>DP33:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="21" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B21" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP25:phraseAgainstPref1_PT</v>
@@ -5902,7 +5902,7 @@
         <v>DP34:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="22" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B22" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP26:phraseAgainstPref1_PT</v>
@@ -5953,7 +5953,7 @@
         <v>DP35:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="23" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B23" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP27:phraseAgainstPref1_PT</v>
@@ -6004,7 +6004,7 @@
         <v>DP36:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="24" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B24" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP28:phraseAgainstPref1_PT</v>
@@ -6013,7 +6013,7 @@
       <c r="H24" s="13"/>
       <c r="J24" s="13"/>
     </row>
-    <row r="25" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B25" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP29:phraseAgainstPref1_PT</v>
@@ -6064,7 +6064,7 @@
         <v>DG1:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="26" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B26" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP30:phraseAgainstPref1_PT</v>
@@ -6115,7 +6115,7 @@
         <v>DG2:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="27" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B27" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP31:phraseAgainstPref1_PT</v>
@@ -6166,7 +6166,7 @@
         <v>DG3:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="28" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B28" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP32:phraseAgainstPref1_PT</v>
@@ -6217,7 +6217,7 @@
         <v>DG5:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="29" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B29" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP33:phraseAgainstPref1_PT</v>
@@ -6268,7 +6268,7 @@
         <v>DG9:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="30" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B30" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP34:phraseAgainstPref1_PT</v>
@@ -6319,7 +6319,7 @@
         <v>DG10:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="31" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B31" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP35:phraseAgainstPref1_PT</v>
@@ -6370,7 +6370,7 @@
         <v>DG11:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="32" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B32" s="8" t="str">
         <f t="shared" si="12"/>
         <v>DP36:phraseAgainstPref1_PT</v>
@@ -6421,7 +6421,7 @@
         <v>DG14:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="33" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B33" s="8" t="str">
         <f>O1</f>
         <v>DP1:phraseAgainstPref2_PT</v>
@@ -6472,25 +6472,25 @@
         <v>DG19:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="34" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B34" s="8" t="str">
         <f t="shared" ref="B34:B55" si="19">O2</f>
         <v>DP2:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="35" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B35" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP3:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="36" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B36" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP4:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="37" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B37" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP5:phraseAgainstPref2_PT</v>
@@ -6501,7 +6501,7 @@
       <c r="P37" s="14"/>
       <c r="Q37" s="14"/>
     </row>
-    <row r="38" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B38" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP6:phraseAgainstPref2_PT</v>
@@ -6512,7 +6512,7 @@
       <c r="P38" s="14"/>
       <c r="Q38" s="14"/>
     </row>
-    <row r="39" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B39" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP7:phraseAgainstPref2_PT</v>
@@ -6523,7 +6523,7 @@
       <c r="P39" s="14"/>
       <c r="Q39" s="14"/>
     </row>
-    <row r="40" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B40" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP10:phraseAgainstPref2_PT</v>
@@ -6534,7 +6534,7 @@
       <c r="P40" s="14"/>
       <c r="Q40" s="14"/>
     </row>
-    <row r="41" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B41" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP11:phraseAgainstPref2_PT</v>
@@ -6545,7 +6545,7 @@
       <c r="P41" s="14"/>
       <c r="Q41" s="14"/>
     </row>
-    <row r="42" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B42" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP12:phraseAgainstPref2_PT</v>
@@ -6556,7 +6556,7 @@
       <c r="P42" s="14"/>
       <c r="Q42" s="14"/>
     </row>
-    <row r="43" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B43" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP18:phraseAgainstPref2_PT</v>
@@ -6567,7 +6567,7 @@
       <c r="P43" s="14"/>
       <c r="Q43" s="14"/>
     </row>
-    <row r="44" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B44" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP25:phraseAgainstPref2_PT</v>
@@ -6578,7 +6578,7 @@
       <c r="P44" s="14"/>
       <c r="Q44" s="14"/>
     </row>
-    <row r="45" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B45" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP26:phraseAgainstPref2_PT</v>
@@ -6589,7 +6589,7 @@
       <c r="P45" s="14"/>
       <c r="Q45" s="14"/>
     </row>
-    <row r="46" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B46" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP27:phraseAgainstPref2_PT</v>
@@ -6600,7 +6600,7 @@
       <c r="P46" s="14"/>
       <c r="Q46" s="14"/>
     </row>
-    <row r="47" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B47" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP28:phraseAgainstPref2_PT</v>
@@ -6611,7 +6611,7 @@
       <c r="P47" s="14"/>
       <c r="Q47" s="14"/>
     </row>
-    <row r="48" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B48" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP29:phraseAgainstPref2_PT</v>
@@ -6622,7 +6622,7 @@
       <c r="P48" s="14"/>
       <c r="Q48" s="14"/>
     </row>
-    <row r="49" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B49" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP30:phraseAgainstPref2_PT</v>
@@ -6633,7 +6633,7 @@
       <c r="P49" s="14"/>
       <c r="Q49" s="14"/>
     </row>
-    <row r="50" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B50" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP31:phraseAgainstPref2_PT</v>
@@ -6644,7 +6644,7 @@
       <c r="P50" s="14"/>
       <c r="Q50" s="14"/>
     </row>
-    <row r="51" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B51" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP32:phraseAgainstPref2_PT</v>
@@ -6655,7 +6655,7 @@
       <c r="P51" s="14"/>
       <c r="Q51" s="14"/>
     </row>
-    <row r="52" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B52" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP33:phraseAgainstPref2_PT</v>
@@ -6666,7 +6666,7 @@
       <c r="P52" s="14"/>
       <c r="Q52" s="14"/>
     </row>
-    <row r="53" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B53" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP34:phraseAgainstPref2_PT</v>
@@ -6677,7 +6677,7 @@
       <c r="P53" s="14"/>
       <c r="Q53" s="14"/>
     </row>
-    <row r="54" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B54" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP35:phraseAgainstPref2_PT</v>
@@ -6688,7 +6688,7 @@
       <c r="P54" s="14"/>
       <c r="Q54" s="14"/>
     </row>
-    <row r="55" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B55" s="8" t="str">
         <f t="shared" si="19"/>
         <v>DP36:phraseAgainstPref2_PT</v>
@@ -6699,7 +6699,7 @@
       <c r="P55" s="14"/>
       <c r="Q55" s="14"/>
     </row>
-    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B56" s="8" t="str">
         <f>Q1</f>
         <v>DP1:phraseFavourPref_PT</v>
@@ -6710,7 +6710,7 @@
       <c r="P56" s="14"/>
       <c r="Q56" s="14"/>
     </row>
-    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B57" s="8" t="str">
         <f t="shared" ref="B57:B78" si="20">Q2</f>
         <v>DP2:phraseFavourPref_PT</v>
@@ -6721,7 +6721,7 @@
       <c r="P57" s="14"/>
       <c r="Q57" s="14"/>
     </row>
-    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B58" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP3:phraseFavourPref_PT</v>
@@ -6732,7 +6732,7 @@
       <c r="P58" s="14"/>
       <c r="Q58" s="14"/>
     </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B59" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP4:phraseFavourPref_PT</v>
@@ -6743,7 +6743,7 @@
       <c r="P59" s="14"/>
       <c r="Q59" s="14"/>
     </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B60" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP5:phraseFavourPref_PT</v>
@@ -6754,7 +6754,7 @@
       <c r="P60" s="14"/>
       <c r="Q60" s="14"/>
     </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B61" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP6:phraseFavourPref_PT</v>
@@ -6765,7 +6765,7 @@
       <c r="P61" s="14"/>
       <c r="Q61" s="14"/>
     </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B62" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP7:phraseFavourPref_PT</v>
@@ -6776,7 +6776,7 @@
       <c r="P62" s="14"/>
       <c r="Q62" s="14"/>
     </row>
-    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B63" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP10:phraseFavourPref_PT</v>
@@ -6787,7 +6787,7 @@
       <c r="P63" s="14"/>
       <c r="Q63" s="14"/>
     </row>
-    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B64" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP11:phraseFavourPref_PT</v>
@@ -6798,7 +6798,7 @@
       <c r="P64" s="14"/>
       <c r="Q64" s="14"/>
     </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B65" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP12:phraseFavourPref_PT</v>
@@ -6809,7 +6809,7 @@
       <c r="P65" s="14"/>
       <c r="Q65" s="14"/>
     </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B66" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP18:phraseFavourPref_PT</v>
@@ -6820,7 +6820,7 @@
       <c r="P66" s="14"/>
       <c r="Q66" s="14"/>
     </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B67" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP25:phraseFavourPref_PT</v>
@@ -6831,7 +6831,7 @@
       <c r="P67" s="14"/>
       <c r="Q67" s="14"/>
     </row>
-    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B68" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP26:phraseFavourPref_PT</v>
@@ -6842,7 +6842,7 @@
       <c r="P68" s="14"/>
       <c r="Q68" s="14"/>
     </row>
-    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B69" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP27:phraseFavourPref_PT</v>
@@ -6853,7 +6853,7 @@
       <c r="P69" s="14"/>
       <c r="Q69" s="14"/>
     </row>
-    <row r="70" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B70" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP28:phraseFavourPref_PT</v>
@@ -6864,7 +6864,7 @@
       <c r="P70" s="14"/>
       <c r="Q70" s="14"/>
     </row>
-    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B71" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP29:phraseFavourPref_PT</v>
@@ -6875,7 +6875,7 @@
       <c r="P71" s="14"/>
       <c r="Q71" s="14"/>
     </row>
-    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B72" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP30:phraseFavourPref_PT</v>
@@ -6886,7 +6886,7 @@
       <c r="P72" s="14"/>
       <c r="Q72" s="14"/>
     </row>
-    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B73" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP31:phraseFavourPref_PT</v>
@@ -6897,7 +6897,7 @@
       <c r="P73" s="14"/>
       <c r="Q73" s="14"/>
     </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B74" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP32:phraseFavourPref_PT</v>
@@ -6908,7 +6908,7 @@
       <c r="P74" s="14"/>
       <c r="Q74" s="14"/>
     </row>
-    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B75" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP33:phraseFavourPref_PT</v>
@@ -6919,7 +6919,7 @@
       <c r="P75" s="14"/>
       <c r="Q75" s="14"/>
     </row>
-    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B76" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP34:phraseFavourPref_PT</v>
@@ -6930,7 +6930,7 @@
       <c r="P76" s="14"/>
       <c r="Q76" s="14"/>
     </row>
-    <row r="77" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B77" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP35:phraseFavourPref_PT</v>
@@ -6941,7 +6941,7 @@
       <c r="P77" s="14"/>
       <c r="Q77" s="14"/>
     </row>
-    <row r="78" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B78" s="8" t="str">
         <f t="shared" si="20"/>
         <v>DP36:phraseFavourPref_PT</v>
@@ -6952,7 +6952,7 @@
       <c r="P78" s="14"/>
       <c r="Q78" s="14"/>
     </row>
-    <row r="79" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B79" s="8" t="str">
         <f>J1</f>
         <v>DP1:phraseAgainstPref1_EN</v>
@@ -6963,7 +6963,7 @@
       <c r="P79" s="14"/>
       <c r="Q79" s="14"/>
     </row>
-    <row r="80" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B80" s="8" t="str">
         <f t="shared" ref="B80:B101" si="21">J2</f>
         <v>DP2:phraseAgainstPref1_EN</v>
@@ -6974,7 +6974,7 @@
       <c r="P80" s="14"/>
       <c r="Q80" s="14"/>
     </row>
-    <row r="81" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B81" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP3:phraseAgainstPref1_EN</v>
@@ -6985,7 +6985,7 @@
       <c r="P81" s="14"/>
       <c r="Q81" s="14"/>
     </row>
-    <row r="82" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B82" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP4:phraseAgainstPref1_EN</v>
@@ -6996,7 +6996,7 @@
       <c r="P82" s="14"/>
       <c r="Q82" s="14"/>
     </row>
-    <row r="83" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B83" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP5:phraseAgainstPref1_EN</v>
@@ -7007,7 +7007,7 @@
       <c r="P83" s="14"/>
       <c r="Q83" s="14"/>
     </row>
-    <row r="84" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B84" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP6:phraseAgainstPref1_EN</v>
@@ -7018,7 +7018,7 @@
       <c r="P84" s="14"/>
       <c r="Q84" s="14"/>
     </row>
-    <row r="85" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B85" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP7:phraseAgainstPref1_EN</v>
@@ -7029,7 +7029,7 @@
       <c r="P85" s="14"/>
       <c r="Q85" s="14"/>
     </row>
-    <row r="86" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B86" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP10:phraseAgainstPref1_EN</v>
@@ -7040,7 +7040,7 @@
       <c r="P86" s="14"/>
       <c r="Q86" s="14"/>
     </row>
-    <row r="87" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B87" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP11:phraseAgainstPref1_EN</v>
@@ -7051,7 +7051,7 @@
       <c r="P87" s="14"/>
       <c r="Q87" s="14"/>
     </row>
-    <row r="88" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B88" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP12:phraseAgainstPref1_EN</v>
@@ -7062,7 +7062,7 @@
       <c r="P88" s="14"/>
       <c r="Q88" s="14"/>
     </row>
-    <row r="89" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B89" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP18:phraseAgainstPref1_EN</v>
@@ -7073,7 +7073,7 @@
       <c r="P89" s="14"/>
       <c r="Q89" s="14"/>
     </row>
-    <row r="90" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B90" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP25:phraseAgainstPref1_EN</v>
@@ -7084,7 +7084,7 @@
       <c r="P90" s="14"/>
       <c r="Q90" s="14"/>
     </row>
-    <row r="91" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B91" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP26:phraseAgainstPref1_EN</v>
@@ -7095,7 +7095,7 @@
       <c r="P91" s="14"/>
       <c r="Q91" s="14"/>
     </row>
-    <row r="92" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B92" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP27:phraseAgainstPref1_EN</v>
@@ -7106,7 +7106,7 @@
       <c r="P92" s="14"/>
       <c r="Q92" s="14"/>
     </row>
-    <row r="93" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B93" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP28:phraseAgainstPref1_EN</v>
@@ -7117,7 +7117,7 @@
       <c r="P93" s="14"/>
       <c r="Q93" s="14"/>
     </row>
-    <row r="94" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B94" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP29:phraseAgainstPref1_EN</v>
@@ -7128,7 +7128,7 @@
       <c r="P94" s="14"/>
       <c r="Q94" s="14"/>
     </row>
-    <row r="95" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B95" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP30:phraseAgainstPref1_EN</v>
@@ -7139,7 +7139,7 @@
       <c r="P95" s="14"/>
       <c r="Q95" s="14"/>
     </row>
-    <row r="96" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B96" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP31:phraseAgainstPref1_EN</v>
@@ -7150,7 +7150,7 @@
       <c r="P96" s="14"/>
       <c r="Q96" s="14"/>
     </row>
-    <row r="97" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B97" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP32:phraseAgainstPref1_EN</v>
@@ -7161,7 +7161,7 @@
       <c r="P97" s="14"/>
       <c r="Q97" s="14"/>
     </row>
-    <row r="98" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B98" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP33:phraseAgainstPref1_EN</v>
@@ -7172,7 +7172,7 @@
       <c r="P98" s="14"/>
       <c r="Q98" s="14"/>
     </row>
-    <row r="99" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B99" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP34:phraseAgainstPref1_EN</v>
@@ -7183,7 +7183,7 @@
       <c r="P99" s="14"/>
       <c r="Q99" s="14"/>
     </row>
-    <row r="100" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B100" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP35:phraseAgainstPref1_EN</v>
@@ -7194,7 +7194,7 @@
       <c r="P100" s="14"/>
       <c r="Q100" s="14"/>
     </row>
-    <row r="101" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B101" s="8" t="str">
         <f t="shared" si="21"/>
         <v>DP36:phraseAgainstPref1_EN</v>
@@ -7205,7 +7205,7 @@
       <c r="P101" s="14"/>
       <c r="Q101" s="14"/>
     </row>
-    <row r="102" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B102" s="8" t="str">
         <f>H1</f>
         <v>DP1:phraseAgainstPref2_EN</v>
@@ -7216,7 +7216,7 @@
       <c r="P102" s="14"/>
       <c r="Q102" s="14"/>
     </row>
-    <row r="103" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B103" s="8" t="str">
         <f t="shared" ref="B103:B124" si="22">H2</f>
         <v>DP2:phraseAgainstPref2_EN</v>
@@ -7227,7 +7227,7 @@
       <c r="P103" s="14"/>
       <c r="Q103" s="14"/>
     </row>
-    <row r="104" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B104" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP3:phraseAgainstPref2_EN</v>
@@ -7238,7 +7238,7 @@
       <c r="P104" s="14"/>
       <c r="Q104" s="14"/>
     </row>
-    <row r="105" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B105" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP4:phraseAgainstPref2_EN</v>
@@ -7249,7 +7249,7 @@
       <c r="P105" s="14"/>
       <c r="Q105" s="14"/>
     </row>
-    <row r="106" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B106" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP5:phraseAgainstPref2_EN</v>
@@ -7260,7 +7260,7 @@
       <c r="P106" s="14"/>
       <c r="Q106" s="14"/>
     </row>
-    <row r="107" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B107" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP6:phraseAgainstPref2_EN</v>
@@ -7271,7 +7271,7 @@
       <c r="P107" s="14"/>
       <c r="Q107" s="14"/>
     </row>
-    <row r="108" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B108" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP7:phraseAgainstPref2_EN</v>
@@ -7282,7 +7282,7 @@
       <c r="P108" s="14"/>
       <c r="Q108" s="14"/>
     </row>
-    <row r="109" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B109" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP10:phraseAgainstPref2_EN</v>
@@ -7293,7 +7293,7 @@
       <c r="P109" s="14"/>
       <c r="Q109" s="14"/>
     </row>
-    <row r="110" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B110" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP11:phraseAgainstPref2_EN</v>
@@ -7304,7 +7304,7 @@
       <c r="P110" s="14"/>
       <c r="Q110" s="14"/>
     </row>
-    <row r="111" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B111" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP12:phraseAgainstPref2_EN</v>
@@ -7315,7 +7315,7 @@
       <c r="P111" s="14"/>
       <c r="Q111" s="14"/>
     </row>
-    <row r="112" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B112" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP18:phraseAgainstPref2_EN</v>
@@ -7326,7 +7326,7 @@
       <c r="P112" s="14"/>
       <c r="Q112" s="14"/>
     </row>
-    <row r="113" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B113" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP25:phraseAgainstPref2_EN</v>
@@ -7337,7 +7337,7 @@
       <c r="P113" s="14"/>
       <c r="Q113" s="14"/>
     </row>
-    <row r="114" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B114" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP26:phraseAgainstPref2_EN</v>
@@ -7348,7 +7348,7 @@
       <c r="P114" s="14"/>
       <c r="Q114" s="14"/>
     </row>
-    <row r="115" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B115" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP27:phraseAgainstPref2_EN</v>
@@ -7359,7 +7359,7 @@
       <c r="P115" s="14"/>
       <c r="Q115" s="14"/>
     </row>
-    <row r="116" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B116" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP28:phraseAgainstPref2_EN</v>
@@ -7370,7 +7370,7 @@
       <c r="P116" s="14"/>
       <c r="Q116" s="14"/>
     </row>
-    <row r="117" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B117" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP29:phraseAgainstPref2_EN</v>
@@ -7381,7 +7381,7 @@
       <c r="P117" s="14"/>
       <c r="Q117" s="14"/>
     </row>
-    <row r="118" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B118" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP30:phraseAgainstPref2_EN</v>
@@ -7392,7 +7392,7 @@
       <c r="P118" s="14"/>
       <c r="Q118" s="14"/>
     </row>
-    <row r="119" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B119" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP31:phraseAgainstPref2_EN</v>
@@ -7403,7 +7403,7 @@
       <c r="P119" s="14"/>
       <c r="Q119" s="14"/>
     </row>
-    <row r="120" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B120" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP32:phraseAgainstPref2_EN</v>
@@ -7414,7 +7414,7 @@
       <c r="P120" s="14"/>
       <c r="Q120" s="14"/>
     </row>
-    <row r="121" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B121" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP33:phraseAgainstPref2_EN</v>
@@ -7425,7 +7425,7 @@
       <c r="P121" s="14"/>
       <c r="Q121" s="14"/>
     </row>
-    <row r="122" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B122" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP34:phraseAgainstPref2_EN</v>
@@ -7436,7 +7436,7 @@
       <c r="P122" s="14"/>
       <c r="Q122" s="14"/>
     </row>
-    <row r="123" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B123" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP35:phraseAgainstPref2_EN</v>
@@ -7447,7 +7447,7 @@
       <c r="P123" s="14"/>
       <c r="Q123" s="14"/>
     </row>
-    <row r="124" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B124" s="8" t="str">
         <f t="shared" si="22"/>
         <v>DP36:phraseAgainstPref2_EN</v>
@@ -7458,7 +7458,7 @@
       <c r="P124" s="14"/>
       <c r="Q124" s="14"/>
     </row>
-    <row r="125" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B125" s="8" t="str">
         <f>F1</f>
         <v>DP1:phraseFavourPref_EN</v>
@@ -7469,7 +7469,7 @@
       <c r="P125" s="14"/>
       <c r="Q125" s="14"/>
     </row>
-    <row r="126" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B126" s="8" t="str">
         <f t="shared" ref="B126:B146" si="23">F2</f>
         <v>DP2:phraseFavourPref_EN</v>
@@ -7480,7 +7480,7 @@
       <c r="P126" s="14"/>
       <c r="Q126" s="14"/>
     </row>
-    <row r="127" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B127" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP3:phraseFavourPref_EN</v>
@@ -7491,7 +7491,7 @@
       <c r="P127" s="14"/>
       <c r="Q127" s="14"/>
     </row>
-    <row r="128" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B128" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP4:phraseFavourPref_EN</v>
@@ -7502,7 +7502,7 @@
       <c r="P128" s="14"/>
       <c r="Q128" s="14"/>
     </row>
-    <row r="129" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B129" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP5:phraseFavourPref_EN</v>
@@ -7513,7 +7513,7 @@
       <c r="P129" s="14"/>
       <c r="Q129" s="14"/>
     </row>
-    <row r="130" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B130" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP6:phraseFavourPref_EN</v>
@@ -7524,7 +7524,7 @@
       <c r="P130" s="14"/>
       <c r="Q130" s="14"/>
     </row>
-    <row r="131" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B131" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP7:phraseFavourPref_EN</v>
@@ -7535,7 +7535,7 @@
       <c r="P131" s="14"/>
       <c r="Q131" s="14"/>
     </row>
-    <row r="132" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B132" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP10:phraseFavourPref_EN</v>
@@ -7546,7 +7546,7 @@
       <c r="P132" s="14"/>
       <c r="Q132" s="14"/>
     </row>
-    <row r="133" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B133" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP11:phraseFavourPref_EN</v>
@@ -7557,7 +7557,7 @@
       <c r="P133" s="14"/>
       <c r="Q133" s="14"/>
     </row>
-    <row r="134" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B134" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP12:phraseFavourPref_EN</v>
@@ -7568,7 +7568,7 @@
       <c r="P134" s="14"/>
       <c r="Q134" s="14"/>
     </row>
-    <row r="135" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B135" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP18:phraseFavourPref_EN</v>
@@ -7579,7 +7579,7 @@
       <c r="P135" s="14"/>
       <c r="Q135" s="14"/>
     </row>
-    <row r="136" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B136" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP25:phraseFavourPref_EN</v>
@@ -7590,7 +7590,7 @@
       <c r="P136" s="14"/>
       <c r="Q136" s="14"/>
     </row>
-    <row r="137" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B137" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP26:phraseFavourPref_EN</v>
@@ -7601,7 +7601,7 @@
       <c r="P137" s="14"/>
       <c r="Q137" s="14"/>
     </row>
-    <row r="138" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B138" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP27:phraseFavourPref_EN</v>
@@ -7612,7 +7612,7 @@
       <c r="P138" s="14"/>
       <c r="Q138" s="14"/>
     </row>
-    <row r="139" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B139" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP28:phraseFavourPref_EN</v>
@@ -7623,7 +7623,7 @@
       <c r="P139" s="14"/>
       <c r="Q139" s="14"/>
     </row>
-    <row r="140" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B140" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP29:phraseFavourPref_EN</v>
@@ -7634,7 +7634,7 @@
       <c r="P140" s="14"/>
       <c r="Q140" s="14"/>
     </row>
-    <row r="141" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B141" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP30:phraseFavourPref_EN</v>
@@ -7645,7 +7645,7 @@
       <c r="P141" s="14"/>
       <c r="Q141" s="14"/>
     </row>
-    <row r="142" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B142" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP31:phraseFavourPref_EN</v>
@@ -7656,7 +7656,7 @@
       <c r="P142" s="14"/>
       <c r="Q142" s="14"/>
     </row>
-    <row r="143" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B143" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP32:phraseFavourPref_EN</v>
@@ -7667,7 +7667,7 @@
       <c r="P143" s="14"/>
       <c r="Q143" s="14"/>
     </row>
-    <row r="144" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B144" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP33:phraseFavourPref_EN</v>
@@ -7678,7 +7678,7 @@
       <c r="P144" s="14"/>
       <c r="Q144" s="14"/>
     </row>
-    <row r="145" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B145" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP34:phraseFavourPref_EN</v>
@@ -7689,7 +7689,7 @@
       <c r="P145" s="14"/>
       <c r="Q145" s="14"/>
     </row>
-    <row r="146" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B146" s="8" t="str">
         <f t="shared" si="23"/>
         <v>DP35:phraseFavourPref_EN</v>
@@ -7700,7 +7700,7 @@
       <c r="P146" s="14"/>
       <c r="Q146" s="14"/>
     </row>
-    <row r="147" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B147" s="8" t="str">
         <f>F23</f>
         <v>DP36:phraseFavourPref_EN</v>
@@ -7711,7 +7711,7 @@
       <c r="P147" s="14"/>
       <c r="Q147" s="14"/>
     </row>
-    <row r="148" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B148" s="8" t="str">
         <f>M25</f>
         <v>DG1:phraseAgainstPref1_PT</v>
@@ -7722,7 +7722,7 @@
       <c r="P148" s="14"/>
       <c r="Q148" s="14"/>
     </row>
-    <row r="149" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B149" s="8" t="str">
         <f t="shared" ref="B149:B156" si="24">M26</f>
         <v>DG2:phraseAgainstPref1_PT</v>
@@ -7733,7 +7733,7 @@
       <c r="P149" s="14"/>
       <c r="Q149" s="14"/>
     </row>
-    <row r="150" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B150" s="8" t="str">
         <f t="shared" si="24"/>
         <v>DG3:phraseAgainstPref1_PT</v>
@@ -7744,7 +7744,7 @@
       <c r="P150" s="14"/>
       <c r="Q150" s="14"/>
     </row>
-    <row r="151" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B151" s="8" t="str">
         <f t="shared" si="24"/>
         <v>DG5:phraseAgainstPref1_PT</v>
@@ -7755,7 +7755,7 @@
       <c r="P151" s="14"/>
       <c r="Q151" s="14"/>
     </row>
-    <row r="152" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B152" s="8" t="str">
         <f t="shared" si="24"/>
         <v>DG9:phraseAgainstPref1_PT</v>
@@ -7766,7 +7766,7 @@
       <c r="P152" s="14"/>
       <c r="Q152" s="14"/>
     </row>
-    <row r="153" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B153" s="8" t="str">
         <f t="shared" si="24"/>
         <v>DG10:phraseAgainstPref1_PT</v>
@@ -7777,7 +7777,7 @@
       <c r="P153" s="14"/>
       <c r="Q153" s="14"/>
     </row>
-    <row r="154" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B154" s="8" t="str">
         <f t="shared" si="24"/>
         <v>DG11:phraseAgainstPref1_PT</v>
@@ -7788,7 +7788,7 @@
       <c r="P154" s="14"/>
       <c r="Q154" s="14"/>
     </row>
-    <row r="155" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B155" s="8" t="str">
         <f t="shared" si="24"/>
         <v>DG14:phraseAgainstPref1_PT</v>
@@ -7799,7 +7799,7 @@
       <c r="P155" s="14"/>
       <c r="Q155" s="14"/>
     </row>
-    <row r="156" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B156" s="8" t="str">
         <f t="shared" si="24"/>
         <v>DG19:phraseAgainstPref1_PT</v>
@@ -7810,7 +7810,7 @@
       <c r="P156" s="14"/>
       <c r="Q156" s="14"/>
     </row>
-    <row r="157" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B157" s="8" t="str">
         <f>O25</f>
         <v>DG1:phraseAgainstPref2_PT</v>
@@ -7821,7 +7821,7 @@
       <c r="P157" s="14"/>
       <c r="Q157" s="14"/>
     </row>
-    <row r="158" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B158" s="8" t="str">
         <f t="shared" ref="B158:B165" si="25">O26</f>
         <v>DG2:phraseAgainstPref2_PT</v>
@@ -7832,259 +7832,259 @@
       <c r="P158" s="14"/>
       <c r="Q158" s="14"/>
     </row>
-    <row r="159" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B159" s="8" t="str">
         <f t="shared" si="25"/>
         <v>DG3:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="160" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B160" s="8" t="str">
         <f t="shared" si="25"/>
         <v>DG5:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="161" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B161" s="8" t="str">
         <f t="shared" si="25"/>
         <v>DG9:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="162" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B162" s="8" t="str">
         <f t="shared" si="25"/>
         <v>DG10:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="163" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B163" s="8" t="str">
         <f t="shared" si="25"/>
         <v>DG11:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="164" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B164" s="8" t="str">
         <f t="shared" si="25"/>
         <v>DG14:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="165" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B165" s="8" t="str">
         <f t="shared" si="25"/>
         <v>DG19:phraseAgainstPref2_PT</v>
       </c>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B166" s="8" t="str">
         <f>Q25</f>
         <v>DG1:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B167" s="8" t="str">
         <f t="shared" ref="B167:B174" si="26">Q26</f>
         <v>DG2:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B168" s="8" t="str">
         <f t="shared" si="26"/>
         <v>DG3:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B169" s="8" t="str">
         <f t="shared" si="26"/>
         <v>DG5:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B170" s="8" t="str">
         <f t="shared" si="26"/>
         <v>DG9:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B171" s="8" t="str">
         <f t="shared" si="26"/>
         <v>DG10:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B172" s="8" t="str">
         <f t="shared" si="26"/>
         <v>DG11:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B173" s="8" t="str">
         <f t="shared" si="26"/>
         <v>DG14:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B174" s="8" t="str">
         <f t="shared" si="26"/>
         <v>DG19:phraseFavourPref_PT</v>
       </c>
     </row>
-    <row r="175" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B175" s="8" t="str">
         <f>J25</f>
         <v>DG1:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="176" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B176" s="8" t="str">
         <f t="shared" ref="B176:B183" si="27">J26</f>
         <v>DG2:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="177" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B177" s="8" t="str">
         <f t="shared" si="27"/>
         <v>DG3:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="178" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B178" s="8" t="str">
         <f t="shared" si="27"/>
         <v>DG5:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="179" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B179" s="8" t="str">
         <f t="shared" si="27"/>
         <v>DG9:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="180" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B180" s="8" t="str">
         <f t="shared" si="27"/>
         <v>DG10:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="181" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B181" s="8" t="str">
         <f t="shared" si="27"/>
         <v>DG11:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="182" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B182" s="8" t="str">
         <f t="shared" si="27"/>
         <v>DG14:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="183" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B183" s="8" t="str">
         <f t="shared" si="27"/>
         <v>DG19:phraseAgainstPref1_EN</v>
       </c>
     </row>
-    <row r="184" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B184" s="8" t="str">
         <f>H25</f>
         <v>DG1:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="185" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B185" s="8" t="str">
         <f t="shared" ref="B185:B192" si="28">H26</f>
         <v>DG2:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="186" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B186" s="8" t="str">
         <f t="shared" si="28"/>
         <v>DG3:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="187" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B187" s="8" t="str">
         <f t="shared" si="28"/>
         <v>DG5:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="188" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B188" s="8" t="str">
         <f t="shared" si="28"/>
         <v>DG9:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="189" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B189" s="8" t="str">
         <f t="shared" si="28"/>
         <v>DG10:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="190" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B190" s="8" t="str">
         <f t="shared" si="28"/>
         <v>DG11:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="191" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B191" s="8" t="str">
         <f t="shared" si="28"/>
         <v>DG14:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="192" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B192" s="8" t="str">
         <f t="shared" si="28"/>
         <v>DG19:phraseAgainstPref2_EN</v>
       </c>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B193" s="8" t="str">
         <f>F25</f>
         <v>DG1:phraseFavourPref_EN</v>
       </c>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B194" s="8" t="str">
         <f t="shared" ref="B194:B200" si="29">F26</f>
         <v>DG2:phraseFavourPref_EN</v>
       </c>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B195" s="8" t="str">
         <f t="shared" si="29"/>
         <v>DG3:phraseFavourPref_EN</v>
       </c>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B196" s="8" t="str">
         <f t="shared" si="29"/>
         <v>DG5:phraseFavourPref_EN</v>
       </c>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B197" s="8" t="str">
         <f t="shared" si="29"/>
         <v>DG9:phraseFavourPref_EN</v>
       </c>
     </row>
-    <row r="198" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B198" s="8" t="str">
         <f t="shared" si="29"/>
         <v>DG10:phraseFavourPref_EN</v>
       </c>
     </row>
-    <row r="199" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B199" s="8" t="str">
         <f t="shared" si="29"/>
         <v>DG11:phraseFavourPref_EN</v>
       </c>
     </row>
-    <row r="200" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B200" s="8" t="str">
         <f t="shared" si="29"/>
         <v>DG14:phraseFavourPref_EN</v>
       </c>
     </row>
-    <row r="201" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B201" s="8" t="str">
         <f>F33</f>
         <v>DG19:phraseFavourPref_EN</v>
@@ -8099,23 +8099,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7405BC36-7328-40C6-8088-275F0F9C1320}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D33"/>
+    <sheetView topLeftCell="D22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="71.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.59765625" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="78" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.85546875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="76.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="69.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="55.140625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="60.86328125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="76.86328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="69.265625" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="55.1328125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -8141,7 +8141,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -8149,10 +8149,10 @@
         <v>11</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>101</v>
@@ -8167,7 +8167,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -8175,7 +8175,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>102</v>
@@ -8193,7 +8193,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -8219,7 +8219,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -8227,7 +8227,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>131</v>
@@ -8245,7 +8245,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -8259,7 +8259,7 @@
         <v>45</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>112</v>
@@ -8271,7 +8271,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -8297,7 +8297,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
@@ -8323,7 +8323,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>7</v>
       </c>
@@ -8349,7 +8349,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>8</v>
       </c>
@@ -8357,7 +8357,7 @@
         <v>21</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>134</v>
@@ -8375,7 +8375,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9</v>
       </c>
@@ -8383,25 +8383,25 @@
         <v>22</v>
       </c>
       <c r="C11" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="E11" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="F11" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="F11" s="16" t="s">
+      <c r="G11" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="H11" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="H11" s="16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>10</v>
       </c>
@@ -8409,25 +8409,25 @@
         <v>23</v>
       </c>
       <c r="C12" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D12" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="E12" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="F12" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="F12" s="16" t="s">
+      <c r="G12" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="H12" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="H12" s="16" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>11</v>
       </c>
@@ -8435,25 +8435,25 @@
         <v>24</v>
       </c>
       <c r="C13" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>149</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>150</v>
       </c>
       <c r="E13" s="16" t="s">
         <v>73</v>
       </c>
       <c r="F13" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="G13" s="16" t="s">
         <v>151</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>152</v>
       </c>
       <c r="H13" s="16" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>12</v>
       </c>
@@ -8461,25 +8461,25 @@
         <v>25</v>
       </c>
       <c r="C14" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="E14" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="F14" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="F14" s="16" t="s">
+      <c r="G14" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="H14" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="H14" s="16" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>13</v>
       </c>
@@ -8487,25 +8487,25 @@
         <v>26</v>
       </c>
       <c r="C15" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="F15" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="G15" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="H15" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="E15" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>14</v>
       </c>
@@ -8513,25 +8513,25 @@
         <v>27</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D16" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="F16" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="F16" s="16" t="s">
+      <c r="G16" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="H16" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="H16" s="16" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" s="15" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A17" s="15">
         <v>15</v>
       </c>
@@ -8539,25 +8539,25 @@
         <v>28</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D17" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="H17" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="E17" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="H17" s="18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>16</v>
       </c>
@@ -8565,25 +8565,25 @@
         <v>29</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D18" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="F18" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="G18" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="H18" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="H18" s="16" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>17</v>
       </c>
@@ -8591,25 +8591,25 @@
         <v>30</v>
       </c>
       <c r="C19" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="D19" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="E19" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="F19" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="G19" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="H19" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="H19" s="16" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>18</v>
       </c>
@@ -8617,25 +8617,25 @@
         <v>31</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E20" s="16" t="s">
         <v>75</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H20" s="16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>19</v>
       </c>
@@ -8643,25 +8643,25 @@
         <v>32</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D21" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="G21" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="E21" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="F21" s="16" t="s">
+      <c r="H21" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="G21" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>20</v>
       </c>
@@ -8669,25 +8669,25 @@
         <v>33</v>
       </c>
       <c r="C22" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="D22" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="E22" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="E22" s="16" t="s">
-        <v>253</v>
-      </c>
-      <c r="F22" s="16" t="s">
+      <c r="G22" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="H22" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="H22" s="16" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>21</v>
       </c>
@@ -8695,25 +8695,25 @@
         <v>34</v>
       </c>
       <c r="C23" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="D23" s="16" t="s">
         <v>195</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>196</v>
       </c>
       <c r="E23" s="16" t="s">
         <v>77</v>
       </c>
       <c r="F23" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="G23" s="16" t="s">
         <v>197</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>198</v>
       </c>
       <c r="H23" s="16" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>22</v>
       </c>
@@ -8721,25 +8721,25 @@
         <v>35</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D24" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="F24" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="G24" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="H24" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="F24" s="16" t="s">
-        <v>200</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="H24" s="16" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>23</v>
       </c>
@@ -8747,25 +8747,25 @@
         <v>43</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E25" s="16" t="s">
         <v>79</v>
       </c>
       <c r="F25" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="G25" s="16" t="s">
         <v>205</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>206</v>
       </c>
       <c r="H25" s="16" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>24</v>
       </c>
@@ -8773,25 +8773,25 @@
         <v>44</v>
       </c>
       <c r="C26" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="F26" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="D26" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="E26" s="16" t="s">
+      <c r="G26" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="H26" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="F26" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>25</v>
       </c>
@@ -8799,25 +8799,25 @@
         <v>46</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F27" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="G27" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="H27" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="H27" s="16" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>26</v>
       </c>
@@ -8825,25 +8825,25 @@
         <v>47</v>
       </c>
       <c r="C28" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="D28" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="E28" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="F28" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="E28" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="F28" s="16" t="s">
+      <c r="G28" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="G28" s="16" t="s">
+      <c r="H28" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="H28" s="16" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>27</v>
       </c>
@@ -8854,22 +8854,22 @@
         <v>64</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F29" s="16" t="s">
         <v>85</v>
       </c>
       <c r="G29" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="H29" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="H29" s="16" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>28</v>
       </c>
@@ -8877,25 +8877,25 @@
         <v>49</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E30" s="16" t="s">
         <v>79</v>
       </c>
       <c r="F30" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="G30" s="16" t="s">
         <v>205</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>206</v>
       </c>
       <c r="H30" s="16" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>29</v>
       </c>
@@ -8903,25 +8903,25 @@
         <v>50</v>
       </c>
       <c r="C31" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="F31" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="G31" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="H31" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="E31" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>30</v>
       </c>
@@ -8947,7 +8947,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>31</v>
       </c>
@@ -8958,19 +8958,19 @@
         <v>64</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F33" s="16" t="s">
         <v>85</v>
       </c>
       <c r="G33" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="H33" s="16" t="s">
         <v>222</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -8990,13 +8990,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="77" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>53</v>
       </c>

</xml_diff>